<commit_message>
Added test and test and set
</commit_message>
<xml_diff>
--- a/src/Speedup Plots.xlsx
+++ b/src/Speedup Plots.xlsx
@@ -234,10 +234,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$7</c:f>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -252,6 +252,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -315,10 +321,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$7</c:f>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -333,6 +339,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -396,10 +408,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$7</c:f>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -414,6 +426,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,10 +495,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$7</c:f>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -495,30 +513,42 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$7</c:f>
+              <c:f>Sheet1!$F$3:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.34974499999999997</c:v>
+                  <c:v>0.47377999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56840500000000005</c:v>
+                  <c:v>1.1694789999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.93152299999999999</c:v>
+                  <c:v>2.2692800000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.560276</c:v>
+                  <c:v>3.0877840000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.991271</c:v>
+                  <c:v>4.2312799999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8675430000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1489589999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -558,10 +588,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$7</c:f>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -576,6 +606,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1011,10 +1047,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$B$13</c:f>
+              <c:f>Sheet1!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1029,13 +1065,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$9:$C$13</c:f>
+              <c:f>Sheet1!$C$11:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1082,9 +1124,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$9:$D$13</c:f>
+              <c:f>Sheet1!$D$11:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1131,9 +1203,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$9:$E$13</c:f>
+              <c:f>Sheet1!$E$11:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1180,26 +1282,62 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$9:$F$13</c:f>
+              <c:f>Sheet1!$F$11:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.339837</c:v>
+                  <c:v>0.32573600000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67490000000000006</c:v>
+                  <c:v>1.572055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1874100000000001</c:v>
+                  <c:v>2.2646269999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.02339</c:v>
+                  <c:v>4.637931</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1421330000000003</c:v>
+                  <c:v>6.574859</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5147779999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2639940000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1229,9 +1367,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$9:$G$13</c:f>
+              <c:f>Sheet1!$G$11:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1665,10 +1833,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1683,13 +1851,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$C$19</c:f>
+              <c:f>Sheet1!$C$19:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1738,10 +1912,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1756,13 +1930,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$15:$D$19</c:f>
+              <c:f>Sheet1!$D$19:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1811,10 +1991,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1829,13 +2009,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$15:$E$19</c:f>
+              <c:f>Sheet1!$E$19:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1884,10 +2070,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1902,30 +2088,42 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$15:$F$19</c:f>
+              <c:f>Sheet1!$F$19:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.36109999999999998</c:v>
+                  <c:v>0.42045199999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45687699999999998</c:v>
+                  <c:v>0.63553499999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73000399999999999</c:v>
+                  <c:v>0.88826000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0507519999999999</c:v>
+                  <c:v>1.3796660000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.221598</c:v>
+                  <c:v>1.8442799999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9492370000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.933767</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1957,10 +2155,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1975,13 +2173,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$15:$G$19</c:f>
+              <c:f>Sheet1!$G$19:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2410,10 +2614,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2428,13 +2632,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$21:$C$25</c:f>
+              <c:f>Sheet1!$C$27:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2483,10 +2693,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2501,13 +2711,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$21:$D$25</c:f>
+              <c:f>Sheet1!$D$27:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2556,10 +2772,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2574,13 +2790,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$21:$E$25</c:f>
+              <c:f>Sheet1!$E$27:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2629,10 +2851,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2647,30 +2869,42 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$21:$F$25</c:f>
+              <c:f>Sheet1!$F$27:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.38574999999999998</c:v>
+                  <c:v>0.41430099999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.627552</c:v>
+                  <c:v>0.59152899999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92106399999999999</c:v>
+                  <c:v>1.066856</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4139250000000001</c:v>
+                  <c:v>1.419103</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.73421</c:v>
+                  <c:v>1.6488499999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6386590000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.654517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2702,10 +2936,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2720,13 +2954,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$21:$G$25</c:f>
+              <c:f>Sheet1!$G$27:$G$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3155,10 +3395,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3173,13 +3413,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$27:$C$31</c:f>
+              <c:f>Sheet1!$C$35:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3228,10 +3474,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3246,13 +3492,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$27:$D$31</c:f>
+              <c:f>Sheet1!$D$35:$D$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3301,10 +3553,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3319,13 +3571,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$27:$E$31</c:f>
+              <c:f>Sheet1!$E$35:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3374,10 +3632,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3392,30 +3650,42 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$27:$F$31</c:f>
+              <c:f>Sheet1!$F$35:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.38025100000000001</c:v>
+                  <c:v>0.45356099999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61681399999999997</c:v>
+                  <c:v>0.847692</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0258879999999999</c:v>
+                  <c:v>1.347421</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5970200000000001</c:v>
+                  <c:v>1.8741129999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.907208</c:v>
+                  <c:v>2.3249240000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3935909999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4026079999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3447,10 +3717,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3465,13 +3735,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$27:$G$31</c:f>
+              <c:f>Sheet1!$G$35:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3900,10 +4176,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3918,13 +4194,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$33:$C$37</c:f>
+              <c:f>Sheet1!$C$43:$C$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3973,10 +4255,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3991,13 +4273,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$33:$D$37</c:f>
+              <c:f>Sheet1!$D$43:$D$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4046,10 +4334,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4064,13 +4352,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$33:$E$37</c:f>
+              <c:f>Sheet1!$E$43:$E$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4119,10 +4413,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4137,30 +4431,42 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$33:$F$37</c:f>
+              <c:f>Sheet1!$F$43:$F$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.35480699999999998</c:v>
+                  <c:v>0.46846100000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.570218</c:v>
+                  <c:v>0.87773500000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.96628599999999998</c:v>
+                  <c:v>1.459373</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3716299999999999</c:v>
+                  <c:v>2.2302949999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.073172</c:v>
+                  <c:v>2.9062380000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9209459999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9717120000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4192,10 +4498,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4210,13 +4516,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$33:$G$37</c:f>
+              <c:f>Sheet1!$G$43:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4645,10 +4957,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$51:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4663,13 +4975,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$C$43</c:f>
+              <c:f>Sheet1!$C$51:$C$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4718,10 +5036,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$51:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4736,13 +5054,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$39:$D$43</c:f>
+              <c:f>Sheet1!$D$51:$D$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4791,10 +5115,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$51:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4809,13 +5133,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$39:$E$43</c:f>
+              <c:f>Sheet1!$E$51:$E$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4864,10 +5194,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$51:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4882,30 +5212,42 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$39:$F$43</c:f>
+              <c:f>Sheet1!$F$51:$F$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.47945599999999999</c:v>
+                  <c:v>0.60749200000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0503629999999999</c:v>
+                  <c:v>0.90420400000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6669659999999999</c:v>
+                  <c:v>1.930709</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9538530000000001</c:v>
+                  <c:v>2.455171</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.065175</c:v>
+                  <c:v>2.65387</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5568140000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5009320000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4937,10 +5279,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$B$19</c:f>
+              <c:f>Sheet1!$B$51:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4955,13 +5297,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$39:$G$43</c:f>
+              <c:f>Sheet1!$G$51:$G$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -9199,7 +9547,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>473868</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9229,13 +9577,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>407193</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9265,13 +9613,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>469106</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>507206</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9301,13 +9649,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>80962</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>119062</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9339,13 +9687,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>490537</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>528637</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9377,13 +9725,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71438</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>109538</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9415,13 +9763,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9749,10 +10097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P59" sqref="P59"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9797,7 +10145,7 @@
         <v>0.77979200000000004</v>
       </c>
       <c r="F3">
-        <v>0.34974499999999997</v>
+        <v>0.47377999999999998</v>
       </c>
       <c r="G3">
         <v>0.16709599999999999</v>
@@ -9817,7 +10165,7 @@
         <v>1.618468</v>
       </c>
       <c r="F4">
-        <v>0.56840500000000005</v>
+        <v>1.1694789999999999</v>
       </c>
       <c r="G4">
         <v>0.27118999999999999</v>
@@ -9837,7 +10185,7 @@
         <v>1.5747150000000001</v>
       </c>
       <c r="F5">
-        <v>0.93152299999999999</v>
+        <v>2.2692800000000002</v>
       </c>
       <c r="G5">
         <v>0.46801300000000001</v>
@@ -9857,7 +10205,7 @@
         <v>1.9567479999999999</v>
       </c>
       <c r="F6">
-        <v>1.560276</v>
+        <v>3.0877840000000001</v>
       </c>
       <c r="G6">
         <v>0.69750199999999996</v>
@@ -9877,324 +10225,269 @@
         <v>3.0352030000000001</v>
       </c>
       <c r="F7">
-        <v>1.991271</v>
+        <v>4.2312799999999999</v>
       </c>
       <c r="G7">
         <v>1.2496430000000001</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <v>4.8675430000000004</v>
+      </c>
+    </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1.0389790000000001</v>
-      </c>
-      <c r="E9">
-        <v>0.88469299999999995</v>
+        <v>64</v>
       </c>
       <c r="F9">
-        <v>0.339837</v>
-      </c>
-      <c r="G9">
-        <v>9.0149000000000007E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1.920083</v>
-      </c>
-      <c r="E10">
-        <v>2.5896729999999999</v>
-      </c>
-      <c r="F10">
-        <v>0.67490000000000006</v>
-      </c>
-      <c r="G10">
-        <v>0.32234400000000002</v>
+        <v>5.1489589999999996</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>2.612174</v>
+        <v>1.0389790000000001</v>
       </c>
       <c r="E11">
-        <v>4.2217149999999997</v>
+        <v>0.88469299999999995</v>
       </c>
       <c r="F11">
-        <v>1.1874100000000001</v>
+        <v>0.32573600000000003</v>
       </c>
       <c r="G11">
-        <v>0.549122</v>
+        <v>9.0149000000000007E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>6.2564469999999996</v>
+        <v>1.920083</v>
       </c>
       <c r="E12">
-        <v>5.5723919999999998</v>
+        <v>2.5896729999999999</v>
       </c>
       <c r="F12">
-        <v>2.02339</v>
+        <v>1.572055</v>
       </c>
       <c r="G12">
-        <v>1.3318110000000001</v>
+        <v>0.32234400000000002</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B13">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>6.9473500000000001</v>
+        <v>2.612174</v>
       </c>
       <c r="E13">
-        <v>9.2813149999999993</v>
+        <v>4.2217149999999997</v>
       </c>
       <c r="F13">
-        <v>4.1421330000000003</v>
+        <v>2.2646269999999999</v>
       </c>
       <c r="G13">
-        <v>1.746254</v>
+        <v>0.549122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>6.2564469999999996</v>
+      </c>
+      <c r="E14">
+        <v>5.5723919999999998</v>
+      </c>
+      <c r="F14">
+        <v>4.637931</v>
+      </c>
+      <c r="G14">
+        <v>1.3318110000000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
       <c r="B15">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0.74416300000000002</v>
+        <v>6.9473500000000001</v>
       </c>
       <c r="E15">
-        <v>0.88520200000000004</v>
+        <v>9.2813149999999993</v>
       </c>
       <c r="F15">
-        <v>0.36109999999999998</v>
+        <v>6.574859</v>
       </c>
       <c r="G15">
-        <v>0.15509000000000001</v>
+        <v>1.746254</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1.0393749999999999</v>
-      </c>
-      <c r="E16">
-        <v>0.954044</v>
+        <v>32</v>
       </c>
       <c r="F16">
-        <v>0.45687699999999998</v>
-      </c>
-      <c r="G16">
-        <v>0.22097</v>
+        <v>7.5147779999999997</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1.5672410000000001</v>
-      </c>
-      <c r="E17">
-        <v>1.526559</v>
+        <v>64</v>
       </c>
       <c r="F17">
-        <v>0.73000399999999999</v>
-      </c>
-      <c r="G17">
-        <v>0.32263700000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>2.4464250000000001</v>
-      </c>
-      <c r="E18">
-        <v>2.4359280000000001</v>
-      </c>
-      <c r="F18">
-        <v>1.0507519999999999</v>
-      </c>
-      <c r="G18">
-        <v>0.47589100000000001</v>
+        <v>8.2639940000000003</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
       <c r="B19">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>4.2575370000000001</v>
+        <v>0.74416300000000002</v>
       </c>
       <c r="E19">
-        <v>4.1169479999999998</v>
+        <v>0.88520200000000004</v>
       </c>
       <c r="F19">
-        <v>1.221598</v>
+        <v>0.42045199999999999</v>
       </c>
       <c r="G19">
-        <v>0.68837499999999996</v>
+        <v>0.15509000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1.0393749999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.954044</v>
+      </c>
+      <c r="F20">
+        <v>0.63553499999999996</v>
+      </c>
+      <c r="G20">
+        <v>0.22097</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
       <c r="B21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0.72842200000000001</v>
+        <v>1.5672410000000001</v>
       </c>
       <c r="E21">
-        <v>0.80843500000000001</v>
+        <v>1.526559</v>
       </c>
       <c r="F21">
-        <v>0.38574999999999998</v>
+        <v>0.88826000000000005</v>
       </c>
       <c r="G21">
-        <v>0.121563</v>
+        <v>0.32263700000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B22">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>1.048678</v>
+        <v>2.4464250000000001</v>
       </c>
       <c r="E22">
-        <v>1.0803769999999999</v>
+        <v>2.4359280000000001</v>
       </c>
       <c r="F22">
-        <v>0.627552</v>
+        <v>1.3796660000000001</v>
       </c>
       <c r="G22">
-        <v>0.221419</v>
+        <v>0.47589100000000001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B23">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>1.599545</v>
+        <v>4.2575370000000001</v>
       </c>
       <c r="E23">
-        <v>2.39384</v>
+        <v>4.1169479999999998</v>
       </c>
       <c r="F23">
-        <v>0.92106399999999999</v>
+        <v>1.8442799999999999</v>
       </c>
       <c r="G23">
-        <v>0.37465500000000002</v>
+        <v>0.68837499999999996</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>2.5808209999999998</v>
-      </c>
-      <c r="E24">
-        <v>2.5846369999999999</v>
+        <v>32</v>
       </c>
       <c r="F24">
-        <v>1.4139250000000001</v>
-      </c>
-      <c r="G24">
-        <v>0.55486599999999997</v>
+        <v>1.9492370000000001</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B25">
-        <v>16</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>4.5462680000000004</v>
-      </c>
-      <c r="E25">
-        <v>4.5530470000000003</v>
+        <v>64</v>
       </c>
       <c r="F25">
-        <v>1.73421</v>
-      </c>
-      <c r="G25">
-        <v>0.88645499999999999</v>
+        <v>1.933767</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -10203,16 +10496,16 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <v>0.70170600000000005</v>
+        <v>0.72842200000000001</v>
       </c>
       <c r="E27">
-        <v>0.75949299999999997</v>
+        <v>0.80843500000000001</v>
       </c>
       <c r="F27">
-        <v>0.38025100000000001</v>
+        <v>0.41430099999999997</v>
       </c>
       <c r="G27">
-        <v>0.14582500000000001</v>
+        <v>0.121563</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
@@ -10223,16 +10516,16 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>1.0476350000000001</v>
+        <v>1.048678</v>
       </c>
       <c r="E28">
-        <v>1.3273539999999999</v>
+        <v>1.0803769999999999</v>
       </c>
       <c r="F28">
-        <v>0.61681399999999997</v>
+        <v>0.59152899999999997</v>
       </c>
       <c r="G28">
-        <v>0.20047999999999999</v>
+        <v>0.221419</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
@@ -10243,16 +10536,16 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>1.6618949999999999</v>
+        <v>1.599545</v>
       </c>
       <c r="E29">
-        <v>1.605118</v>
+        <v>2.39384</v>
       </c>
       <c r="F29">
-        <v>1.0258879999999999</v>
+        <v>1.066856</v>
       </c>
       <c r="G29">
-        <v>0.34470400000000001</v>
+        <v>0.37465500000000002</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
@@ -10263,16 +10556,16 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>2.7392110000000001</v>
+        <v>2.5808209999999998</v>
       </c>
       <c r="E30">
-        <v>2.6796959999999999</v>
+        <v>2.5846369999999999</v>
       </c>
       <c r="F30">
-        <v>1.5970200000000001</v>
+        <v>1.419103</v>
       </c>
       <c r="G30">
-        <v>0.56314399999999998</v>
+        <v>0.55486599999999997</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
@@ -10283,222 +10576,389 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>3.634331</v>
+        <v>4.5462680000000004</v>
       </c>
       <c r="E31">
-        <v>4.0432569999999997</v>
+        <v>4.5530470000000003</v>
       </c>
       <c r="F31">
-        <v>1.907208</v>
+        <v>1.6488499999999999</v>
       </c>
       <c r="G31">
-        <v>0.90338300000000005</v>
+        <v>0.88645499999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>32</v>
+      </c>
+      <c r="F32">
+        <v>1.6386590000000001</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
       <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>0.84155199999999997</v>
-      </c>
-      <c r="E33">
-        <v>0.89085800000000004</v>
+        <v>64</v>
       </c>
       <c r="F33">
-        <v>0.35480699999999998</v>
-      </c>
-      <c r="G33">
-        <v>0.127917</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>1.3051360000000001</v>
-      </c>
-      <c r="E34">
-        <v>1.2307490000000001</v>
-      </c>
-      <c r="F34">
-        <v>0.570218</v>
-      </c>
-      <c r="G34">
-        <v>0.25795600000000002</v>
+        <v>1.654517</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
       <c r="B35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>2.0754899999999998</v>
+        <v>0.70170600000000005</v>
       </c>
       <c r="E35">
-        <v>2.0229529999999998</v>
+        <v>0.75949299999999997</v>
       </c>
       <c r="F35">
-        <v>0.96628599999999998</v>
+        <v>0.45356099999999999</v>
       </c>
       <c r="G35">
-        <v>0.413823</v>
+        <v>0.14582500000000001</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B36">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36">
-        <v>3.470059</v>
+        <v>1.0476350000000001</v>
       </c>
       <c r="E36">
-        <v>3.4853969999999999</v>
+        <v>1.3273539999999999</v>
       </c>
       <c r="F36">
-        <v>1.3716299999999999</v>
+        <v>0.847692</v>
       </c>
       <c r="G36">
-        <v>0.682118</v>
+        <v>0.20047999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B37">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>5.9494889999999998</v>
+        <v>1.6618949999999999</v>
       </c>
       <c r="E37">
-        <v>5.820837</v>
+        <v>1.605118</v>
       </c>
       <c r="F37">
-        <v>2.073172</v>
+        <v>1.347421</v>
       </c>
       <c r="G37">
-        <v>0.89427400000000001</v>
+        <v>0.34470400000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>2.7392110000000001</v>
+      </c>
+      <c r="E38">
+        <v>2.6796959999999999</v>
+      </c>
+      <c r="F38">
+        <v>1.8741129999999999</v>
+      </c>
+      <c r="G38">
+        <v>0.56314399999999998</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>5</v>
-      </c>
       <c r="B39">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39">
-        <v>0.52261100000000005</v>
+        <v>3.634331</v>
       </c>
       <c r="E39">
-        <v>0.74985199999999996</v>
+        <v>4.0432569999999997</v>
       </c>
       <c r="F39">
-        <v>0.47945599999999999</v>
+        <v>2.3249240000000002</v>
       </c>
       <c r="G39">
-        <v>0.13525300000000001</v>
+        <v>0.90338300000000005</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>0.84881499999999999</v>
-      </c>
-      <c r="E40">
-        <v>1.415635</v>
+        <v>32</v>
       </c>
       <c r="F40">
-        <v>1.0503629999999999</v>
-      </c>
-      <c r="G40">
-        <v>0.22179199999999999</v>
+        <v>2.3935909999999998</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B41">
-        <v>4</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1.3893789999999999</v>
-      </c>
-      <c r="E41">
-        <v>2.2003729999999999</v>
+        <v>64</v>
       </c>
       <c r="F41">
-        <v>1.6669659999999999</v>
-      </c>
-      <c r="G41">
-        <v>0.35908299999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B42">
-        <v>8</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>2.3360560000000001</v>
-      </c>
-      <c r="E42">
-        <v>2.312252</v>
-      </c>
-      <c r="F42">
-        <v>2.9538530000000001</v>
-      </c>
-      <c r="G42">
-        <v>0.56882900000000003</v>
+        <v>2.4026079999999999</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
       <c r="B43">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43">
+        <v>0.84155199999999997</v>
+      </c>
+      <c r="E43">
+        <v>0.89085800000000004</v>
+      </c>
+      <c r="F43">
+        <v>0.46846100000000002</v>
+      </c>
+      <c r="G43">
+        <v>0.127917</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1.3051360000000001</v>
+      </c>
+      <c r="E44">
+        <v>1.2307490000000001</v>
+      </c>
+      <c r="F44">
+        <v>0.87773500000000004</v>
+      </c>
+      <c r="G44">
+        <v>0.25795600000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>2.0754899999999998</v>
+      </c>
+      <c r="E45">
+        <v>2.0229529999999998</v>
+      </c>
+      <c r="F45">
+        <v>1.459373</v>
+      </c>
+      <c r="G45">
+        <v>0.413823</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>3.470059</v>
+      </c>
+      <c r="E46">
+        <v>3.4853969999999999</v>
+      </c>
+      <c r="F46">
+        <v>2.2302949999999999</v>
+      </c>
+      <c r="G46">
+        <v>0.682118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B47">
+        <v>16</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>5.9494889999999998</v>
+      </c>
+      <c r="E47">
+        <v>5.820837</v>
+      </c>
+      <c r="F47">
+        <v>2.9062380000000001</v>
+      </c>
+      <c r="G47">
+        <v>0.89427400000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B48">
+        <v>32</v>
+      </c>
+      <c r="F48">
+        <v>2.9209459999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B49">
+        <v>64</v>
+      </c>
+      <c r="F49">
+        <v>2.9717120000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0.52261100000000005</v>
+      </c>
+      <c r="E51">
+        <v>0.74985199999999996</v>
+      </c>
+      <c r="F51">
+        <v>0.60749200000000003</v>
+      </c>
+      <c r="G51">
+        <v>0.13525300000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0.84881499999999999</v>
+      </c>
+      <c r="E52">
+        <v>1.415635</v>
+      </c>
+      <c r="F52">
+        <v>0.90420400000000001</v>
+      </c>
+      <c r="G52">
+        <v>0.22179199999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1.3893789999999999</v>
+      </c>
+      <c r="E53">
+        <v>2.2003729999999999</v>
+      </c>
+      <c r="F53">
+        <v>1.930709</v>
+      </c>
+      <c r="G53">
+        <v>0.35908299999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B54">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>2.3360560000000001</v>
+      </c>
+      <c r="E54">
+        <v>2.312252</v>
+      </c>
+      <c r="F54">
+        <v>2.455171</v>
+      </c>
+      <c r="G54">
+        <v>0.56882900000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B55">
+        <v>16</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
         <v>3.349634</v>
       </c>
-      <c r="E43">
+      <c r="E55">
         <v>4.24756</v>
       </c>
-      <c r="F43">
-        <v>4.065175</v>
-      </c>
-      <c r="G43">
+      <c r="F55">
+        <v>2.65387</v>
+      </c>
+      <c r="G55">
         <v>0.82408099999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B56">
+        <v>32</v>
+      </c>
+      <c r="F56">
+        <v>2.5568140000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B57">
+        <v>64</v>
+      </c>
+      <c r="F57">
+        <v>2.5009320000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new fine grained, lock free, and hazard ptr times to excel
</commit_message>
<xml_diff>
--- a/src/Speedup Plots.xlsx
+++ b/src/Speedup Plots.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4075eb16eb3fe1a6/Documents/Sophomore Year/15-418/Term Project/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18825" windowHeight="12308"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -68,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +125,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -171,6 +169,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -179,26 +178,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -239,25 +218,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -269,25 +248,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E8B6-4EE0-A1F6-E380067B43EC}"/>
             </c:ext>
@@ -326,25 +305,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -356,25 +335,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.610792</c:v>
+                  <c:v>0.735319</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97460599999999997</c:v>
+                  <c:v>1.380216</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.563464</c:v>
+                  <c:v>2.568034</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6509999999999998</c:v>
+                  <c:v>3.260371</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.602468</c:v>
+                  <c:v>2.717456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E8B6-4EE0-A1F6-E380067B43EC}"/>
             </c:ext>
@@ -413,25 +392,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -443,25 +422,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.77979200000000004</c:v>
+                  <c:v>0.694564</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.618468</c:v>
+                  <c:v>1.311903</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5747150000000001</c:v>
+                  <c:v>2.464281</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9567479999999999</c:v>
+                  <c:v>3.304003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0352030000000001</c:v>
+                  <c:v>2.674274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-E8B6-4EE0-A1F6-E380067B43EC}"/>
             </c:ext>
@@ -500,25 +479,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,31 +509,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.47377999999999998</c:v>
+                  <c:v>0.47378</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1694789999999999</c:v>
+                  <c:v>1.169479</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2692800000000002</c:v>
+                  <c:v>2.26928</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0877840000000001</c:v>
+                  <c:v>3.087784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2312799999999999</c:v>
+                  <c:v>4.23128</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8675430000000004</c:v>
+                  <c:v>4.867543</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.1489589999999996</c:v>
+                  <c:v>5.148959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-E8B6-4EE0-A1F6-E380067B43EC}"/>
             </c:ext>
@@ -593,25 +572,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -623,25 +602,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.16709599999999999</c:v>
+                  <c:v>0.272845</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27118999999999999</c:v>
+                  <c:v>0.467366</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46801300000000001</c:v>
+                  <c:v>0.762378</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69750199999999996</c:v>
+                  <c:v>1.303177</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2496430000000001</c:v>
+                  <c:v>1.88478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-E8B6-4EE0-A1F6-E380067B43EC}"/>
             </c:ext>
@@ -655,12 +634,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="435626288"/>
-        <c:axId val="435626616"/>
+        <c:axId val="2128546488"/>
+        <c:axId val="2128182472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="435626288"/>
+        <c:axId val="2128546488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,6 +672,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -700,26 +681,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -758,7 +719,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="435626616"/>
+        <c:crossAx val="2128182472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -766,7 +727,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="435626616"/>
+        <c:axId val="2128182472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,6 +773,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -820,26 +782,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -872,7 +814,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="435626288"/>
+        <c:crossAx val="2128546488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -886,6 +828,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -953,7 +896,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -992,6 +935,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1000,26 +944,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1052,25 +976,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,25 +1006,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000016-6734-4567-A374-2717DB571389}"/>
             </c:ext>
@@ -1131,25 +1055,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1161,25 +1085,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.0389790000000001</c:v>
+                  <c:v>1.082989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.920083</c:v>
+                  <c:v>6.908236</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.612174</c:v>
+                  <c:v>9.059282</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2564469999999996</c:v>
+                  <c:v>20.751224</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.9473500000000001</c:v>
+                  <c:v>23.666299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000017-6734-4567-A374-2717DB571389}"/>
             </c:ext>
@@ -1210,25 +1134,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1240,25 +1164,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.88469299999999995</c:v>
+                  <c:v>0.94789</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5896729999999999</c:v>
+                  <c:v>4.874127</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2217149999999997</c:v>
+                  <c:v>7.623686</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.5723919999999998</c:v>
+                  <c:v>18.026693</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2813149999999993</c:v>
+                  <c:v>18.331176</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000018-6734-4567-A374-2717DB571389}"/>
             </c:ext>
@@ -1289,25 +1213,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1319,13 +1243,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.32573600000000003</c:v>
+                  <c:v>0.325736</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.572055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2646269999999999</c:v>
+                  <c:v>2.264627</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4.637931</c:v>
@@ -1334,16 +1258,16 @@
                   <c:v>6.574859</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5147779999999997</c:v>
+                  <c:v>7.514778</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2639940000000003</c:v>
+                  <c:v>8.263994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000019-6734-4567-A374-2717DB571389}"/>
             </c:ext>
@@ -1374,25 +1298,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,25 +1328,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.0149000000000007E-2</c:v>
+                  <c:v>0.281329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32234400000000002</c:v>
+                  <c:v>1.087811</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.549122</c:v>
+                  <c:v>2.065527</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3318110000000001</c:v>
+                  <c:v>3.511884</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.746254</c:v>
+                  <c:v>6.080603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001A-6734-4567-A374-2717DB571389}"/>
             </c:ext>
@@ -1436,12 +1360,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="584592976"/>
-        <c:axId val="584599536"/>
+        <c:axId val="2123017880"/>
+        <c:axId val="2123276312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="584592976"/>
+        <c:axId val="2123017880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,6 +1403,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1486,26 +1412,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1544,7 +1450,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="584599536"/>
+        <c:crossAx val="2123276312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1552,7 +1458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="584599536"/>
+        <c:axId val="2123276312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1598,6 +1504,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1606,26 +1513,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1658,7 +1545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="584592976"/>
+        <c:crossAx val="2123017880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1672,6 +1559,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1739,7 +1627,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1778,6 +1666,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1786,26 +1675,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1838,25 +1707,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1868,25 +1737,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0E66-43B9-9A3F-D9484BB3BD9E}"/>
             </c:ext>
@@ -1917,25 +1786,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1947,25 +1816,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.74416300000000002</c:v>
+                  <c:v>0.954634</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0393749999999999</c:v>
+                  <c:v>1.381688</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5672410000000001</c:v>
+                  <c:v>2.599911</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4464250000000001</c:v>
+                  <c:v>3.891794</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2575370000000001</c:v>
+                  <c:v>3.580818</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0E66-43B9-9A3F-D9484BB3BD9E}"/>
             </c:ext>
@@ -1996,25 +1865,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2026,25 +1895,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.88520200000000004</c:v>
+                  <c:v>0.788484</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.954044</c:v>
+                  <c:v>1.344242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.526559</c:v>
+                  <c:v>2.471514</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4359280000000001</c:v>
+                  <c:v>2.651593</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1169479999999998</c:v>
+                  <c:v>3.612736</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0E66-43B9-9A3F-D9484BB3BD9E}"/>
             </c:ext>
@@ -2075,25 +1944,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2105,22 +1974,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.42045199999999999</c:v>
+                  <c:v>0.420452</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63553499999999996</c:v>
+                  <c:v>0.635535</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88826000000000005</c:v>
+                  <c:v>0.88826</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3796660000000001</c:v>
+                  <c:v>1.379666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8442799999999999</c:v>
+                  <c:v>1.84428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9492370000000001</c:v>
+                  <c:v>1.949237</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.933767</c:v>
@@ -2129,7 +1998,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-0E66-43B9-9A3F-D9484BB3BD9E}"/>
             </c:ext>
@@ -2160,25 +2029,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2190,25 +2059,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.15509000000000001</c:v>
+                  <c:v>0.210478</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22097</c:v>
+                  <c:v>0.255637</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32263700000000001</c:v>
+                  <c:v>0.415112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47589100000000001</c:v>
+                  <c:v>0.668143</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.68837499999999996</c:v>
+                  <c:v>1.034841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-0E66-43B9-9A3F-D9484BB3BD9E}"/>
             </c:ext>
@@ -2222,12 +2091,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="448364800"/>
-        <c:axId val="448365128"/>
+        <c:axId val="2123023928"/>
+        <c:axId val="2127739352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448364800"/>
+        <c:axId val="2123023928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2259,6 +2129,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2267,26 +2138,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2325,7 +2176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448365128"/>
+        <c:crossAx val="2127739352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2333,7 +2184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448365128"/>
+        <c:axId val="2127739352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2379,6 +2230,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2387,26 +2239,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2439,7 +2271,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448364800"/>
+        <c:crossAx val="2123023928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2453,6 +2285,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2520,7 +2353,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2559,6 +2392,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2567,26 +2401,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2619,25 +2433,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2649,25 +2463,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-04D1-4A7A-A03C-708D7A2D7D9F}"/>
             </c:ext>
@@ -2698,25 +2512,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2728,25 +2542,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.72842200000000001</c:v>
+                  <c:v>1.003777</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.048678</c:v>
+                  <c:v>1.683553</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.599545</c:v>
+                  <c:v>2.771625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5808209999999998</c:v>
+                  <c:v>3.086535</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5462680000000004</c:v>
+                  <c:v>1.699752</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-04D1-4A7A-A03C-708D7A2D7D9F}"/>
             </c:ext>
@@ -2777,25 +2591,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2807,25 +2621,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.80843500000000001</c:v>
+                  <c:v>0.901171</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0803769999999999</c:v>
+                  <c:v>1.521083</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.39384</c:v>
+                  <c:v>2.699475</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5846369999999999</c:v>
+                  <c:v>5.148271</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5530470000000003</c:v>
+                  <c:v>6.09521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-04D1-4A7A-A03C-708D7A2D7D9F}"/>
             </c:ext>
@@ -2856,25 +2670,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2886,10 +2700,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.41430099999999997</c:v>
+                  <c:v>0.414301</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59152899999999997</c:v>
+                  <c:v>0.591529</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.066856</c:v>
@@ -2898,10 +2712,10 @@
                   <c:v>1.419103</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6488499999999999</c:v>
+                  <c:v>1.64885</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6386590000000001</c:v>
+                  <c:v>1.638659</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.654517</c:v>
@@ -2910,7 +2724,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-04D1-4A7A-A03C-708D7A2D7D9F}"/>
             </c:ext>
@@ -2941,25 +2755,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2971,25 +2785,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.121563</c:v>
+                  <c:v>0.267635</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.221419</c:v>
+                  <c:v>0.395969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37465500000000002</c:v>
+                  <c:v>0.708247</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55486599999999997</c:v>
+                  <c:v>1.012136</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.88645499999999999</c:v>
+                  <c:v>1.525165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-04D1-4A7A-A03C-708D7A2D7D9F}"/>
             </c:ext>
@@ -3003,12 +2817,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="448364800"/>
-        <c:axId val="448365128"/>
+        <c:axId val="2128556456"/>
+        <c:axId val="2123041032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448364800"/>
+        <c:axId val="2128556456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3040,6 +2855,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3048,26 +2864,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3106,7 +2902,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448365128"/>
+        <c:crossAx val="2123041032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3114,7 +2910,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448365128"/>
+        <c:axId val="2123041032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3160,6 +2956,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3168,26 +2965,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3220,7 +2997,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448364800"/>
+        <c:crossAx val="2128556456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3234,6 +3011,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3301,7 +3079,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3340,6 +3118,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3348,26 +3127,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3400,25 +3159,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3430,25 +3189,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-81A1-4718-9640-86A65D7ABFED}"/>
             </c:ext>
@@ -3479,25 +3238,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3509,25 +3268,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.70170600000000005</c:v>
+                  <c:v>0.957858</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0476350000000001</c:v>
+                  <c:v>1.441053</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6618949999999999</c:v>
+                  <c:v>4.261493</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7392110000000001</c:v>
+                  <c:v>7.809296</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.634331</c:v>
+                  <c:v>7.566273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-81A1-4718-9640-86A65D7ABFED}"/>
             </c:ext>
@@ -3558,25 +3317,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3588,25 +3347,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.75949299999999997</c:v>
+                  <c:v>1.030745</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3273539999999999</c:v>
+                  <c:v>1.997586</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.605118</c:v>
+                  <c:v>3.19719</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6796959999999999</c:v>
+                  <c:v>5.323648</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0432569999999997</c:v>
+                  <c:v>8.555474</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-81A1-4718-9640-86A65D7ABFED}"/>
             </c:ext>
@@ -3637,25 +3396,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3667,7 +3426,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.45356099999999999</c:v>
+                  <c:v>0.453561</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.847692</c:v>
@@ -3676,22 +3435,22 @@
                   <c:v>1.347421</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8741129999999999</c:v>
+                  <c:v>1.874113</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3249240000000002</c:v>
+                  <c:v>2.324924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3935909999999998</c:v>
+                  <c:v>2.393591</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4026079999999999</c:v>
+                  <c:v>2.402608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-81A1-4718-9640-86A65D7ABFED}"/>
             </c:ext>
@@ -3722,25 +3481,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3752,25 +3511,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.14582500000000001</c:v>
+                  <c:v>0.285523</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20047999999999999</c:v>
+                  <c:v>0.454941</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34470400000000001</c:v>
+                  <c:v>0.733057</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56314399999999998</c:v>
+                  <c:v>1.417312</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90338300000000005</c:v>
+                  <c:v>1.933101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-81A1-4718-9640-86A65D7ABFED}"/>
             </c:ext>
@@ -3784,12 +3543,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="448364800"/>
-        <c:axId val="448365128"/>
+        <c:axId val="2123736296"/>
+        <c:axId val="2094294536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448364800"/>
+        <c:axId val="2123736296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3821,6 +3581,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3829,26 +3590,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3887,7 +3628,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448365128"/>
+        <c:crossAx val="2094294536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3895,7 +3636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448365128"/>
+        <c:axId val="2094294536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3941,6 +3682,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3949,26 +3691,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4001,7 +3723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448364800"/>
+        <c:crossAx val="2123736296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4015,6 +3737,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4082,7 +3805,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4129,26 +3852,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4181,25 +3884,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4211,25 +3914,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8004-4C32-BB46-3C3042542D70}"/>
             </c:ext>
@@ -4260,25 +3963,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4290,25 +3993,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.84155199999999997</c:v>
+                  <c:v>0.975188</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3051360000000001</c:v>
+                  <c:v>2.036376</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0754899999999998</c:v>
+                  <c:v>3.323208</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.470059</c:v>
+                  <c:v>5.607928</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.9494889999999998</c:v>
+                  <c:v>9.75671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8004-4C32-BB46-3C3042542D70}"/>
             </c:ext>
@@ -4339,25 +4042,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4369,25 +4072,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.89085800000000004</c:v>
+                  <c:v>0.895467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2307490000000001</c:v>
+                  <c:v>1.606464</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0229529999999998</c:v>
+                  <c:v>3.242197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4853969999999999</c:v>
+                  <c:v>5.411716</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.820837</c:v>
+                  <c:v>9.784809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-8004-4C32-BB46-3C3042542D70}"/>
             </c:ext>
@@ -4418,25 +4121,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4448,31 +4151,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.46846100000000002</c:v>
+                  <c:v>0.468461</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.87773500000000004</c:v>
+                  <c:v>0.877735</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.459373</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2302949999999999</c:v>
+                  <c:v>2.230295</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9062380000000001</c:v>
+                  <c:v>2.906238</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9209459999999998</c:v>
+                  <c:v>2.920946</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9717120000000001</c:v>
+                  <c:v>2.971712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-8004-4C32-BB46-3C3042542D70}"/>
             </c:ext>
@@ -4503,25 +4206,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4533,25 +4236,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.127917</c:v>
+                  <c:v>0.304575</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25795600000000002</c:v>
+                  <c:v>0.491189</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.413823</c:v>
+                  <c:v>0.857583</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.682118</c:v>
+                  <c:v>1.483814</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.89427400000000001</c:v>
+                  <c:v>2.210994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-8004-4C32-BB46-3C3042542D70}"/>
             </c:ext>
@@ -4565,12 +4268,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="448364800"/>
-        <c:axId val="448365128"/>
+        <c:axId val="2140564504"/>
+        <c:axId val="2140571128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448364800"/>
+        <c:axId val="2140564504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4610,26 +4314,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4668,7 +4352,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448365128"/>
+        <c:crossAx val="2140571128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4676,7 +4360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448365128"/>
+        <c:axId val="2140571128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4730,26 +4414,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4782,7 +4446,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448364800"/>
+        <c:crossAx val="2140564504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4863,7 +4527,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4910,26 +4574,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4962,25 +4606,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4992,25 +4636,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9399-45B5-9EC6-725E04CDF974}"/>
             </c:ext>
@@ -5041,25 +4685,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5071,25 +4715,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.52261100000000005</c:v>
+                  <c:v>0.906523</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.84881499999999999</c:v>
+                  <c:v>1.642932</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3893789999999999</c:v>
+                  <c:v>2.832087</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3360560000000001</c:v>
+                  <c:v>4.122037</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.349634</c:v>
+                  <c:v>4.288915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9399-45B5-9EC6-725E04CDF974}"/>
             </c:ext>
@@ -5120,25 +4764,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5150,25 +4794,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.74985199999999996</c:v>
+                  <c:v>0.774994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.415635</c:v>
+                  <c:v>1.544046</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2003729999999999</c:v>
+                  <c:v>2.16049</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.312252</c:v>
+                  <c:v>4.091751</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.24756</c:v>
+                  <c:v>5.152546</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-9399-45B5-9EC6-725E04CDF974}"/>
             </c:ext>
@@ -5199,25 +4843,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5229,10 +4873,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.60749200000000003</c:v>
+                  <c:v>0.607492</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90420400000000001</c:v>
+                  <c:v>0.904204</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.930709</c:v>
@@ -5244,16 +4888,16 @@
                   <c:v>2.65387</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5568140000000001</c:v>
+                  <c:v>2.556814</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5009320000000002</c:v>
+                  <c:v>2.500932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-9399-45B5-9EC6-725E04CDF974}"/>
             </c:ext>
@@ -5284,25 +4928,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5314,25 +4958,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.13525300000000001</c:v>
+                  <c:v>0.211183</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22179199999999999</c:v>
+                  <c:v>0.416922</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35908299999999999</c:v>
+                  <c:v>0.565755</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56882900000000003</c:v>
+                  <c:v>1.05627</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.82408099999999995</c:v>
+                  <c:v>1.560004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-9399-45B5-9EC6-725E04CDF974}"/>
             </c:ext>
@@ -5346,12 +4990,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="448364800"/>
-        <c:axId val="448365128"/>
+        <c:axId val="2130480728"/>
+        <c:axId val="2130617656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448364800"/>
+        <c:axId val="2130480728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5391,26 +5036,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -5449,7 +5074,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448365128"/>
+        <c:crossAx val="2130617656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5457,7 +5082,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448365128"/>
+        <c:axId val="2130617656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5511,26 +5136,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -5563,7 +5168,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448364800"/>
+        <c:crossAx val="2130480728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9555,7 +9160,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51012497-131E-438D-A4EC-857E05081FE8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51012497-131E-438D-A4EC-857E05081FE8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9591,7 +9196,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{841B80DB-1658-4214-B585-0D4F5C6F8DD3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{841B80DB-1658-4214-B585-0D4F5C6F8DD3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9627,7 +9232,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABF21383-498A-4642-A2CB-835C8BE05BF9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABF21383-498A-4642-A2CB-835C8BE05BF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9663,7 +9268,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93B70A89-6039-47BC-A03A-89D46F09A368}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93B70A89-6039-47BC-A03A-89D46F09A368}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9701,7 +9306,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C2FA1F-171E-4F71-A85C-86192FB26C8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C2FA1F-171E-4F71-A85C-86192FB26C8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9739,7 +9344,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95F1A27D-5B75-4BFC-BB52-BCB4D036EB7A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95F1A27D-5B75-4BFC-BB52-BCB4D036EB7A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9777,7 +9382,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F35E7B1-41A7-4330-A0BD-4E589BA3A1C1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F35E7B1-41A7-4330-A0BD-4E589BA3A1C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9843,7 +9448,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -9895,7 +9500,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -10089,7 +9694,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10099,19 +9704,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7">
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
@@ -10128,7 +9733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -10139,19 +9744,19 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.610792</v>
+        <v>0.73531899999999994</v>
       </c>
       <c r="E3">
-        <v>0.77979200000000004</v>
+        <v>0.69456399999999996</v>
       </c>
       <c r="F3">
         <v>0.47377999999999998</v>
       </c>
       <c r="G3">
-        <v>0.16709599999999999</v>
+        <v>0.272845</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7">
       <c r="B4">
         <v>2</v>
       </c>
@@ -10159,19 +9764,19 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.97460599999999997</v>
+        <v>1.3802160000000001</v>
       </c>
       <c r="E4">
-        <v>1.618468</v>
+        <v>1.311903</v>
       </c>
       <c r="F4">
         <v>1.1694789999999999</v>
       </c>
       <c r="G4">
-        <v>0.27118999999999999</v>
+        <v>0.467366</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7">
       <c r="B5">
         <v>4</v>
       </c>
@@ -10179,19 +9784,19 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1.563464</v>
+        <v>2.5680339999999999</v>
       </c>
       <c r="E5">
-        <v>1.5747150000000001</v>
+        <v>2.4642810000000002</v>
       </c>
       <c r="F5">
         <v>2.2692800000000002</v>
       </c>
       <c r="G5">
-        <v>0.46801300000000001</v>
+        <v>0.762378</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7">
       <c r="B6">
         <v>8</v>
       </c>
@@ -10199,19 +9804,19 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>2.6509999999999998</v>
+        <v>3.2603710000000001</v>
       </c>
       <c r="E6">
-        <v>1.9567479999999999</v>
+        <v>3.3040029999999998</v>
       </c>
       <c r="F6">
         <v>3.0877840000000001</v>
       </c>
       <c r="G6">
-        <v>0.69750199999999996</v>
+        <v>1.303177</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7">
       <c r="B7">
         <v>16</v>
       </c>
@@ -10219,35 +9824,59 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>3.602468</v>
+        <v>2.7174559999999999</v>
       </c>
       <c r="E7">
-        <v>3.0352030000000001</v>
+        <v>2.674274</v>
       </c>
       <c r="F7">
         <v>4.2312799999999999</v>
       </c>
       <c r="G7">
-        <v>1.2496430000000001</v>
+        <v>1.8847799999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7">
       <c r="B8">
         <v>32</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2.6841539999999999</v>
+      </c>
+      <c r="E8">
+        <v>2.5400779999999998</v>
+      </c>
       <c r="F8">
         <v>4.8675430000000004</v>
       </c>
+      <c r="G8">
+        <v>2.2061579999999998</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7">
       <c r="B9">
         <v>64</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2.4920179999999998</v>
+      </c>
+      <c r="E9">
+        <v>2.4246460000000001</v>
+      </c>
       <c r="F9">
         <v>5.1489589999999996</v>
       </c>
+      <c r="G9">
+        <v>2.2929840000000001</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -10258,19 +9887,19 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1.0389790000000001</v>
+        <v>1.082989</v>
       </c>
       <c r="E11">
-        <v>0.88469299999999995</v>
+        <v>0.94789000000000001</v>
       </c>
       <c r="F11">
         <v>0.32573600000000003</v>
       </c>
       <c r="G11">
-        <v>9.0149000000000007E-2</v>
+        <v>0.281329</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7">
       <c r="B12">
         <v>2</v>
       </c>
@@ -10278,19 +9907,19 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>1.920083</v>
+        <v>6.9082359999999996</v>
       </c>
       <c r="E12">
-        <v>2.5896729999999999</v>
+        <v>4.8741269999999997</v>
       </c>
       <c r="F12">
         <v>1.572055</v>
       </c>
       <c r="G12">
-        <v>0.32234400000000002</v>
+        <v>1.0878110000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7">
       <c r="B13">
         <v>4</v>
       </c>
@@ -10298,19 +9927,19 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>2.612174</v>
+        <v>9.0592819999999996</v>
       </c>
       <c r="E13">
-        <v>4.2217149999999997</v>
+        <v>7.6236860000000002</v>
       </c>
       <c r="F13">
         <v>2.2646269999999999</v>
       </c>
       <c r="G13">
-        <v>0.549122</v>
+        <v>2.0655269999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7">
       <c r="B14">
         <v>8</v>
       </c>
@@ -10318,19 +9947,19 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>6.2564469999999996</v>
+        <v>20.751224000000001</v>
       </c>
       <c r="E14">
-        <v>5.5723919999999998</v>
+        <v>18.026693000000002</v>
       </c>
       <c r="F14">
         <v>4.637931</v>
       </c>
       <c r="G14">
-        <v>1.3318110000000001</v>
+        <v>3.5118839999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7">
       <c r="B15">
         <v>16</v>
       </c>
@@ -10338,35 +9967,59 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>6.9473500000000001</v>
+        <v>23.666298999999999</v>
       </c>
       <c r="E15">
-        <v>9.2813149999999993</v>
+        <v>18.331175999999999</v>
       </c>
       <c r="F15">
         <v>6.574859</v>
       </c>
       <c r="G15">
-        <v>1.746254</v>
+        <v>6.080603</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7">
       <c r="B16">
         <v>32</v>
       </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>22.651153000000001</v>
+      </c>
+      <c r="E16">
+        <v>24.481449999999999</v>
+      </c>
       <c r="F16">
         <v>7.5147779999999997</v>
       </c>
+      <c r="G16">
+        <v>7.754365</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7">
       <c r="B17">
         <v>64</v>
       </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>17.046006999999999</v>
+      </c>
+      <c r="E17">
+        <v>17.006654999999999</v>
+      </c>
       <c r="F17">
         <v>8.2639940000000003</v>
       </c>
+      <c r="G17">
+        <v>7.6610620000000003</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -10377,19 +10030,19 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>0.74416300000000002</v>
+        <v>0.95463399999999998</v>
       </c>
       <c r="E19">
-        <v>0.88520200000000004</v>
+        <v>0.78848399999999996</v>
       </c>
       <c r="F19">
         <v>0.42045199999999999</v>
       </c>
       <c r="G19">
-        <v>0.15509000000000001</v>
+        <v>0.210478</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7">
       <c r="B20">
         <v>2</v>
       </c>
@@ -10397,19 +10050,19 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>1.0393749999999999</v>
+        <v>1.381688</v>
       </c>
       <c r="E20">
-        <v>0.954044</v>
+        <v>1.3442419999999999</v>
       </c>
       <c r="F20">
         <v>0.63553499999999996</v>
       </c>
       <c r="G20">
-        <v>0.22097</v>
+        <v>0.255637</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7">
       <c r="B21">
         <v>4</v>
       </c>
@@ -10417,19 +10070,19 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>1.5672410000000001</v>
+        <v>2.5999110000000001</v>
       </c>
       <c r="E21">
-        <v>1.526559</v>
+        <v>2.471514</v>
       </c>
       <c r="F21">
         <v>0.88826000000000005</v>
       </c>
       <c r="G21">
-        <v>0.32263700000000001</v>
+        <v>0.41511199999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7">
       <c r="B22">
         <v>8</v>
       </c>
@@ -10437,19 +10090,19 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>2.4464250000000001</v>
+        <v>3.891794</v>
       </c>
       <c r="E22">
-        <v>2.4359280000000001</v>
+        <v>2.6515930000000001</v>
       </c>
       <c r="F22">
         <v>1.3796660000000001</v>
       </c>
       <c r="G22">
-        <v>0.47589100000000001</v>
+        <v>0.66814300000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7">
       <c r="B23">
         <v>16</v>
       </c>
@@ -10457,35 +10110,59 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>4.2575370000000001</v>
+        <v>3.5808179999999998</v>
       </c>
       <c r="E23">
-        <v>4.1169479999999998</v>
+        <v>3.6127359999999999</v>
       </c>
       <c r="F23">
         <v>1.8442799999999999</v>
       </c>
       <c r="G23">
-        <v>0.68837499999999996</v>
+        <v>1.0348409999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7">
       <c r="B24">
         <v>32</v>
       </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>3.438555</v>
+      </c>
+      <c r="E24">
+        <v>3.3925930000000002</v>
+      </c>
       <c r="F24">
         <v>1.9492370000000001</v>
       </c>
+      <c r="G24">
+        <v>1.2176119999999999</v>
+      </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7">
       <c r="B25">
         <v>64</v>
       </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>3.4086120000000002</v>
+      </c>
+      <c r="E25">
+        <v>3.3514279999999999</v>
+      </c>
       <c r="F25">
         <v>1.933767</v>
       </c>
+      <c r="G25">
+        <v>1.2788809999999999</v>
+      </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -10496,19 +10173,19 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <v>0.72842200000000001</v>
+        <v>1.0037769999999999</v>
       </c>
       <c r="E27">
-        <v>0.80843500000000001</v>
+        <v>0.90117100000000006</v>
       </c>
       <c r="F27">
         <v>0.41430099999999997</v>
       </c>
       <c r="G27">
-        <v>0.121563</v>
+        <v>0.26763500000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7">
       <c r="B28">
         <v>2</v>
       </c>
@@ -10516,19 +10193,19 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>1.048678</v>
+        <v>1.6835530000000001</v>
       </c>
       <c r="E28">
-        <v>1.0803769999999999</v>
+        <v>1.521083</v>
       </c>
       <c r="F28">
         <v>0.59152899999999997</v>
       </c>
       <c r="G28">
-        <v>0.221419</v>
+        <v>0.39596900000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7">
       <c r="B29">
         <v>4</v>
       </c>
@@ -10536,19 +10213,19 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>1.599545</v>
+        <v>2.7716249999999998</v>
       </c>
       <c r="E29">
-        <v>2.39384</v>
+        <v>2.6994750000000001</v>
       </c>
       <c r="F29">
         <v>1.066856</v>
       </c>
       <c r="G29">
-        <v>0.37465500000000002</v>
+        <v>0.70824699999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7">
       <c r="B30">
         <v>8</v>
       </c>
@@ -10556,19 +10233,19 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>2.5808209999999998</v>
+        <v>3.086535</v>
       </c>
       <c r="E30">
-        <v>2.5846369999999999</v>
+        <v>5.1482710000000003</v>
       </c>
       <c r="F30">
         <v>1.419103</v>
       </c>
       <c r="G30">
-        <v>0.55486599999999997</v>
+        <v>1.0121359999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7">
       <c r="B31">
         <v>16</v>
       </c>
@@ -10576,35 +10253,59 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>4.5462680000000004</v>
+        <v>1.6997519999999999</v>
       </c>
       <c r="E31">
-        <v>4.5530470000000003</v>
+        <v>6.0952099999999998</v>
       </c>
       <c r="F31">
         <v>1.6488499999999999</v>
       </c>
       <c r="G31">
-        <v>0.88645499999999999</v>
+        <v>1.5251650000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7">
       <c r="B32">
         <v>32</v>
       </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>5.3962630000000003</v>
+      </c>
+      <c r="E32">
+        <v>5.4977980000000004</v>
+      </c>
       <c r="F32">
         <v>1.6386590000000001</v>
       </c>
+      <c r="G32">
+        <v>1.7468429999999999</v>
+      </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7">
       <c r="B33">
         <v>64</v>
       </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>5.796875</v>
+      </c>
+      <c r="E33">
+        <v>5.6038990000000002</v>
+      </c>
       <c r="F33">
         <v>1.654517</v>
       </c>
+      <c r="G33">
+        <v>1.8672359999999999</v>
+      </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -10615,19 +10316,19 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>0.70170600000000005</v>
+        <v>0.95785799999999999</v>
       </c>
       <c r="E35">
-        <v>0.75949299999999997</v>
+        <v>1.030745</v>
       </c>
       <c r="F35">
         <v>0.45356099999999999</v>
       </c>
       <c r="G35">
-        <v>0.14582500000000001</v>
+        <v>0.28552300000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7">
       <c r="B36">
         <v>2</v>
       </c>
@@ -10635,19 +10336,19 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <v>1.0476350000000001</v>
+        <v>1.4410529999999999</v>
       </c>
       <c r="E36">
-        <v>1.3273539999999999</v>
+        <v>1.9975860000000001</v>
       </c>
       <c r="F36">
         <v>0.847692</v>
       </c>
       <c r="G36">
-        <v>0.20047999999999999</v>
+        <v>0.45494099999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7">
       <c r="B37">
         <v>4</v>
       </c>
@@ -10655,19 +10356,19 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <v>1.6618949999999999</v>
+        <v>4.2614929999999998</v>
       </c>
       <c r="E37">
-        <v>1.605118</v>
+        <v>3.19719</v>
       </c>
       <c r="F37">
         <v>1.347421</v>
       </c>
       <c r="G37">
-        <v>0.34470400000000001</v>
+        <v>0.73305699999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7">
       <c r="B38">
         <v>8</v>
       </c>
@@ -10675,19 +10376,19 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>2.7392110000000001</v>
+        <v>7.8092959999999998</v>
       </c>
       <c r="E38">
-        <v>2.6796959999999999</v>
+        <v>5.3236480000000004</v>
       </c>
       <c r="F38">
         <v>1.8741129999999999</v>
       </c>
       <c r="G38">
-        <v>0.56314399999999998</v>
+        <v>1.4173119999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7">
       <c r="B39">
         <v>16</v>
       </c>
@@ -10695,35 +10396,59 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <v>3.634331</v>
+        <v>7.5662729999999998</v>
       </c>
       <c r="E39">
-        <v>4.0432569999999997</v>
+        <v>8.5554740000000002</v>
       </c>
       <c r="F39">
         <v>2.3249240000000002</v>
       </c>
       <c r="G39">
-        <v>0.90338300000000005</v>
+        <v>1.933101</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7">
       <c r="B40">
         <v>32</v>
       </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>5.7097449999999998</v>
+      </c>
+      <c r="E40">
+        <v>7.5459800000000001</v>
+      </c>
       <c r="F40">
         <v>2.3935909999999998</v>
       </c>
+      <c r="G40">
+        <v>2.168488</v>
+      </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7">
       <c r="B41">
         <v>64</v>
       </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>5.6901380000000001</v>
+      </c>
+      <c r="E41">
+        <v>8.220618</v>
+      </c>
       <c r="F41">
         <v>2.4026079999999999</v>
       </c>
+      <c r="G41">
+        <v>2.4301780000000002</v>
+      </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -10734,19 +10459,19 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <v>0.84155199999999997</v>
+        <v>0.97518800000000005</v>
       </c>
       <c r="E43">
-        <v>0.89085800000000004</v>
+        <v>0.89546700000000001</v>
       </c>
       <c r="F43">
         <v>0.46846100000000002</v>
       </c>
       <c r="G43">
-        <v>0.127917</v>
+        <v>0.30457499999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7">
       <c r="B44">
         <v>2</v>
       </c>
@@ -10754,19 +10479,19 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <v>1.3051360000000001</v>
+        <v>2.0363760000000002</v>
       </c>
       <c r="E44">
-        <v>1.2307490000000001</v>
+        <v>1.6064639999999999</v>
       </c>
       <c r="F44">
         <v>0.87773500000000004</v>
       </c>
       <c r="G44">
-        <v>0.25795600000000002</v>
+        <v>0.49118899999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7">
       <c r="B45">
         <v>4</v>
       </c>
@@ -10774,19 +10499,19 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <v>2.0754899999999998</v>
+        <v>3.3232080000000002</v>
       </c>
       <c r="E45">
-        <v>2.0229529999999998</v>
+        <v>3.242197</v>
       </c>
       <c r="F45">
         <v>1.459373</v>
       </c>
       <c r="G45">
-        <v>0.413823</v>
+        <v>0.85758299999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7">
       <c r="B46">
         <v>8</v>
       </c>
@@ -10794,19 +10519,19 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>3.470059</v>
+        <v>5.6079280000000002</v>
       </c>
       <c r="E46">
-        <v>3.4853969999999999</v>
+        <v>5.4117160000000002</v>
       </c>
       <c r="F46">
         <v>2.2302949999999999</v>
       </c>
       <c r="G46">
-        <v>0.682118</v>
+        <v>1.483814</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7">
       <c r="B47">
         <v>16</v>
       </c>
@@ -10814,35 +10539,59 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <v>5.9494889999999998</v>
+        <v>9.75671</v>
       </c>
       <c r="E47">
-        <v>5.820837</v>
+        <v>9.7848089999999992</v>
       </c>
       <c r="F47">
         <v>2.9062380000000001</v>
       </c>
       <c r="G47">
-        <v>0.89427400000000001</v>
+        <v>2.2109939999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7">
       <c r="B48">
         <v>32</v>
       </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>8.0020399999999992</v>
+      </c>
+      <c r="E48">
+        <v>7.7783129999999998</v>
+      </c>
       <c r="F48">
         <v>2.9209459999999998</v>
       </c>
+      <c r="G48">
+        <v>2.3715860000000002</v>
+      </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7">
       <c r="B49">
         <v>64</v>
       </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>9.3039970000000007</v>
+      </c>
+      <c r="E49">
+        <v>8.3077749999999995</v>
+      </c>
       <c r="F49">
         <v>2.9717120000000001</v>
       </c>
+      <c r="G49">
+        <v>2.3917609999999998</v>
+      </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -10853,19 +10602,19 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <v>0.52261100000000005</v>
+        <v>0.90652299999999997</v>
       </c>
       <c r="E51">
-        <v>0.74985199999999996</v>
+        <v>0.77499399999999996</v>
       </c>
       <c r="F51">
         <v>0.60749200000000003</v>
       </c>
       <c r="G51">
-        <v>0.13525300000000001</v>
+        <v>0.21118300000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7">
       <c r="B52">
         <v>2</v>
       </c>
@@ -10873,19 +10622,19 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>0.84881499999999999</v>
+        <v>1.6429320000000001</v>
       </c>
       <c r="E52">
-        <v>1.415635</v>
+        <v>1.544046</v>
       </c>
       <c r="F52">
         <v>0.90420400000000001</v>
       </c>
       <c r="G52">
-        <v>0.22179199999999999</v>
+        <v>0.41692200000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7">
       <c r="B53">
         <v>4</v>
       </c>
@@ -10893,19 +10642,19 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>1.3893789999999999</v>
+        <v>2.832087</v>
       </c>
       <c r="E53">
-        <v>2.2003729999999999</v>
+        <v>2.1604899999999998</v>
       </c>
       <c r="F53">
         <v>1.930709</v>
       </c>
       <c r="G53">
-        <v>0.35908299999999999</v>
+        <v>0.56575500000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7">
       <c r="B54">
         <v>8</v>
       </c>
@@ -10913,19 +10662,19 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <v>2.3360560000000001</v>
+        <v>4.1220369999999997</v>
       </c>
       <c r="E54">
-        <v>2.312252</v>
+        <v>4.0917510000000004</v>
       </c>
       <c r="F54">
         <v>2.455171</v>
       </c>
       <c r="G54">
-        <v>0.56882900000000003</v>
+        <v>1.05627</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7">
       <c r="B55">
         <v>16</v>
       </c>
@@ -10933,37 +10682,66 @@
         <v>1</v>
       </c>
       <c r="D55">
-        <v>3.349634</v>
+        <v>4.2889150000000003</v>
       </c>
       <c r="E55">
-        <v>4.24756</v>
+        <v>5.1525460000000001</v>
       </c>
       <c r="F55">
         <v>2.65387</v>
       </c>
       <c r="G55">
-        <v>0.82408099999999995</v>
+        <v>1.5600039999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7">
       <c r="B56">
         <v>32</v>
       </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>2.8816700000000002</v>
+      </c>
+      <c r="E56">
+        <v>3.6952319999999999</v>
+      </c>
       <c r="F56">
         <v>2.5568140000000001</v>
       </c>
+      <c r="G56">
+        <v>1.625758</v>
+      </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7">
       <c r="B57">
         <v>64</v>
       </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>3.6626430000000001</v>
+      </c>
+      <c r="E57">
+        <v>3.4673240000000001</v>
+      </c>
       <c r="F57">
         <v>2.5009320000000002</v>
+      </c>
+      <c r="G57">
+        <v>1.696807</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added load factor cpp test file
</commit_message>
<xml_diff>
--- a/src/Speedup Plots.xlsx
+++ b/src/Speedup Plots.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="25600" windowHeight="14800"/>
+    <workbookView xWindow="13760" yWindow="0" windowWidth="25600" windowHeight="14800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>30% Delete</t>
   </si>
@@ -64,6 +65,24 @@
   </si>
   <si>
     <t>10% del 10% ins</t>
+  </si>
+  <si>
+    <t>load_factor_test.txt</t>
+  </si>
+  <si>
+    <t>load factor: 1</t>
+  </si>
+  <si>
+    <t>load factor: 5</t>
+  </si>
+  <si>
+    <t>load factor: 10</t>
+  </si>
+  <si>
+    <t>load factor: 15</t>
+  </si>
+  <si>
+    <t>load factor: 20</t>
   </si>
 </sst>
 </file>
@@ -120,8 +139,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -135,15 +158,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -753,11 +780,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2128062824"/>
-        <c:axId val="2127834232"/>
+        <c:axId val="2145538152"/>
+        <c:axId val="2145546744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2128062824"/>
+        <c:axId val="2145538152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -838,13 +865,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127834232"/>
+        <c:crossAx val="2145546744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2127834232"/>
+        <c:axId val="2145546744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128062824"/>
+        <c:crossAx val="2145538152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1561,11 +1588,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2124504680"/>
-        <c:axId val="2125193912"/>
+        <c:axId val="2145606536"/>
+        <c:axId val="2143488904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2124504680"/>
+        <c:axId val="2145606536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -1645,13 +1672,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125193912"/>
+        <c:crossAx val="2143488904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2125193912"/>
+        <c:axId val="2143488904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,7 +1765,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124504680"/>
+        <c:crossAx val="2145606536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2368,11 +2395,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141715080"/>
-        <c:axId val="2141976584"/>
+        <c:axId val="2145964888"/>
+        <c:axId val="2145973416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141715080"/>
+        <c:axId val="2145964888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -2452,13 +2479,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141976584"/>
+        <c:crossAx val="2145973416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141976584"/>
+        <c:axId val="2145973416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,7 +2572,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141715080"/>
+        <c:crossAx val="2145964888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3175,11 +3202,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142022568"/>
-        <c:axId val="2142031192"/>
+        <c:axId val="2146158344"/>
+        <c:axId val="2146166872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142022568"/>
+        <c:axId val="2146158344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -3259,13 +3286,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142031192"/>
+        <c:crossAx val="2146166872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142031192"/>
+        <c:axId val="2146166872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3352,7 +3379,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142022568"/>
+        <c:crossAx val="2146158344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3982,11 +4009,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142068328"/>
-        <c:axId val="2142076952"/>
+        <c:axId val="2146203528"/>
+        <c:axId val="2146212056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142068328"/>
+        <c:axId val="2146203528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -4066,13 +4093,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142076952"/>
+        <c:crossAx val="2146212056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142076952"/>
+        <c:axId val="2146212056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4159,7 +4186,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142068328"/>
+        <c:crossAx val="2146203528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4789,11 +4816,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2127673944"/>
-        <c:axId val="2139337240"/>
+        <c:axId val="2143741512"/>
+        <c:axId val="2145461672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2127673944"/>
+        <c:axId val="2143741512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -4873,13 +4900,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2139337240"/>
+        <c:crossAx val="2145461672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2139337240"/>
+        <c:axId val="2145461672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4966,7 +4993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127673944"/>
+        <c:crossAx val="2143741512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8403,7 +8430,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{51012497-131E-438D-A4EC-857E05081FE8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51012497-131E-438D-A4EC-857E05081FE8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8439,7 +8466,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ABF21383-498A-4642-A2CB-835C8BE05BF9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABF21383-498A-4642-A2CB-835C8BE05BF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8475,7 +8502,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{93B70A89-6039-47BC-A03A-89D46F09A368}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93B70A89-6039-47BC-A03A-89D46F09A368}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8513,7 +8540,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D9C2FA1F-171E-4F71-A85C-86192FB26C8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C2FA1F-171E-4F71-A85C-86192FB26C8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8551,7 +8578,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{95F1A27D-5B75-4BFC-BB52-BCB4D036EB7A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95F1A27D-5B75-4BFC-BB52-BCB4D036EB7A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8589,7 +8616,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F35E7B1-41A7-4330-A0BD-4E589BA3A1C1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F35E7B1-41A7-4330-A0BD-4E589BA3A1C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8901,7 +8928,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8911,8 +8938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10055,4 +10082,557 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.84029799999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.75723399999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1.506165</v>
+      </c>
+      <c r="E4">
+        <v>1.370449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1.656131</v>
+      </c>
+      <c r="E5">
+        <v>2.0372750000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2.822292</v>
+      </c>
+      <c r="E6">
+        <v>3.5110980000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>3.56602</v>
+      </c>
+      <c r="E7">
+        <v>3.9436779999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2.932604</v>
+      </c>
+      <c r="E8">
+        <v>3.0300910000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9">
+        <v>64</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2.740246</v>
+      </c>
+      <c r="E9">
+        <v>2.7802980000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0.89391600000000004</v>
+      </c>
+      <c r="E11">
+        <v>0.77187700000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1.512775</v>
+      </c>
+      <c r="E12">
+        <v>1.2931170000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2.456906</v>
+      </c>
+      <c r="E13">
+        <v>2.2189830000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>3.3306469999999999</v>
+      </c>
+      <c r="E14">
+        <v>3.2570480000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>4.1716889999999998</v>
+      </c>
+      <c r="E15">
+        <v>4.2766229999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>3.2779739999999999</v>
+      </c>
+      <c r="E16">
+        <v>3.1607340000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17">
+        <v>64</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2.759865</v>
+      </c>
+      <c r="E17">
+        <v>2.8426230000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0.87892199999999998</v>
+      </c>
+      <c r="E19">
+        <v>0.79469800000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1.468933</v>
+      </c>
+      <c r="E20">
+        <v>1.43045</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2.4531100000000001</v>
+      </c>
+      <c r="E21">
+        <v>2.484308</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>3.8334139999999999</v>
+      </c>
+      <c r="E22">
+        <v>3.6984430000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>4.619192</v>
+      </c>
+      <c r="E23">
+        <v>4.9700810000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>3.393856</v>
+      </c>
+      <c r="E24">
+        <v>3.369523</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25">
+        <v>64</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>3.3242289999999999</v>
+      </c>
+      <c r="E25">
+        <v>3.047879</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0.95079999999999998</v>
+      </c>
+      <c r="E27">
+        <v>0.87454799999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1.5674939999999999</v>
+      </c>
+      <c r="E28">
+        <v>1.4436150000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>2.59043</v>
+      </c>
+      <c r="E29">
+        <v>2.5623870000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>3.7209810000000001</v>
+      </c>
+      <c r="E30">
+        <v>3.2183929999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>4.770651</v>
+      </c>
+      <c r="E31">
+        <v>4.7530599999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32">
+        <v>32</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>3.550468</v>
+      </c>
+      <c r="E32">
+        <v>3.4933740000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="B33">
+        <v>64</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>3.407346</v>
+      </c>
+      <c r="E33">
+        <v>3.1794690000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1.0066619999999999</v>
+      </c>
+      <c r="E35">
+        <v>0.84752000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1.649076</v>
+      </c>
+      <c r="E36">
+        <v>1.564548</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>2.795048</v>
+      </c>
+      <c r="E37">
+        <v>2.6789260000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>4.1241890000000003</v>
+      </c>
+      <c r="E38">
+        <v>4.1311869999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="B39">
+        <v>16</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>5.0794160000000002</v>
+      </c>
+      <c r="E39">
+        <v>6.0910450000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="B40">
+        <v>32</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>3.8361320000000001</v>
+      </c>
+      <c r="E40">
+        <v>3.7800600000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="B41">
+        <v>64</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>3.68445</v>
+      </c>
+      <c r="E41">
+        <v>3.5267590000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Load Factor speedups missing hazptr
</commit_message>
<xml_diff>
--- a/src/Speedup Plots.xlsx
+++ b/src/Speedup Plots.xlsx
@@ -6721,25 +6721,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.48161399999999999</c:v>
+                  <c:v>0.43965500000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.84786300000000003</c:v>
+                  <c:v>0.79086900000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.446753</c:v>
+                  <c:v>1.42069</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9671179999999999</c:v>
+                  <c:v>1.837367</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9432689999999999</c:v>
+                  <c:v>1.9172210000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9125559999999999</c:v>
+                  <c:v>1.903195</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9091959999999999</c:v>
+                  <c:v>1.9467669999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12203,7 +12203,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -12250,6 +12252,9 @@
       <c r="E3">
         <v>0.75723399999999996</v>
       </c>
+      <c r="F3">
+        <v>0.28692299999999998</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B4">
@@ -12264,6 +12269,9 @@
       <c r="E4">
         <v>1.370449</v>
       </c>
+      <c r="F4">
+        <v>0.44977200000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5">
@@ -12278,6 +12286,9 @@
       <c r="E5">
         <v>2.0372750000000002</v>
       </c>
+      <c r="F5">
+        <v>0.55448299999999995</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6">
@@ -12292,6 +12303,9 @@
       <c r="E6">
         <v>3.5110980000000001</v>
       </c>
+      <c r="F6">
+        <v>0.70880799999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7">
@@ -12306,6 +12320,9 @@
       <c r="E7">
         <v>3.9436779999999998</v>
       </c>
+      <c r="F7">
+        <v>0.71130199999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8">
@@ -12320,6 +12337,9 @@
       <c r="E8">
         <v>3.0300910000000001</v>
       </c>
+      <c r="F8">
+        <v>0.717916</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9">
@@ -12334,6 +12354,9 @@
       <c r="E9">
         <v>2.7802980000000002</v>
       </c>
+      <c r="F9">
+        <v>0.71992500000000004</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -12351,6 +12374,9 @@
       <c r="E11">
         <v>0.77187700000000004</v>
       </c>
+      <c r="F11">
+        <v>0.55763499999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12">
@@ -12365,6 +12391,9 @@
       <c r="E12">
         <v>1.2931170000000001</v>
       </c>
+      <c r="F12">
+        <v>0.73817500000000003</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B13">
@@ -12379,6 +12408,9 @@
       <c r="E13">
         <v>2.2189830000000001</v>
       </c>
+      <c r="F13">
+        <v>1.215751</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B14">
@@ -12393,6 +12425,9 @@
       <c r="E14">
         <v>3.2570480000000002</v>
       </c>
+      <c r="F14">
+        <v>1.302767</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B15">
@@ -12407,6 +12442,9 @@
       <c r="E15">
         <v>4.2766229999999998</v>
       </c>
+      <c r="F15">
+        <v>1.2324790000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B16">
@@ -12421,8 +12459,11 @@
       <c r="E16">
         <v>3.1607340000000002</v>
       </c>
+      <c r="F16">
+        <v>1.2296640000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>64</v>
       </c>
@@ -12435,8 +12476,11 @@
       <c r="E17">
         <v>2.8426230000000001</v>
       </c>
+      <c r="F17">
+        <v>1.205122</v>
+      </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -12452,8 +12496,11 @@
       <c r="E19">
         <v>0.79469800000000002</v>
       </c>
+      <c r="F19">
+        <v>0.37883600000000001</v>
+      </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>2</v>
       </c>
@@ -12466,8 +12513,11 @@
       <c r="E20">
         <v>1.43045</v>
       </c>
+      <c r="F20">
+        <v>0.59200399999999997</v>
+      </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>4</v>
       </c>
@@ -12480,8 +12530,11 @@
       <c r="E21">
         <v>2.484308</v>
       </c>
+      <c r="F21">
+        <v>0.874089</v>
+      </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>8</v>
       </c>
@@ -12494,8 +12547,11 @@
       <c r="E22">
         <v>3.6984430000000001</v>
       </c>
+      <c r="F22">
+        <v>0.90456199999999998</v>
+      </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>16</v>
       </c>
@@ -12508,8 +12564,11 @@
       <c r="E23">
         <v>4.9700810000000004</v>
       </c>
+      <c r="F23">
+        <v>0.91234599999999999</v>
+      </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>32</v>
       </c>
@@ -12522,8 +12581,11 @@
       <c r="E24">
         <v>3.369523</v>
       </c>
+      <c r="F24">
+        <v>0.91863600000000001</v>
+      </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>64</v>
       </c>
@@ -12536,8 +12598,11 @@
       <c r="E25">
         <v>3.047879</v>
       </c>
+      <c r="F25">
+        <v>0.92056300000000002</v>
+      </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -12553,8 +12618,11 @@
       <c r="E27">
         <v>0.87454799999999999</v>
       </c>
+      <c r="F27">
+        <v>0.41204000000000002</v>
+      </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>2</v>
       </c>
@@ -12567,8 +12635,11 @@
       <c r="E28">
         <v>1.4436150000000001</v>
       </c>
+      <c r="F28">
+        <v>0.51643099999999997</v>
+      </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>4</v>
       </c>
@@ -12581,8 +12652,11 @@
       <c r="E29">
         <v>2.5623870000000002</v>
       </c>
+      <c r="F29">
+        <v>0.75488599999999995</v>
+      </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>8</v>
       </c>
@@ -12595,8 +12669,11 @@
       <c r="E30">
         <v>3.2183929999999998</v>
       </c>
+      <c r="F30">
+        <v>0.98655000000000004</v>
+      </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>16</v>
       </c>
@@ -12609,8 +12686,11 @@
       <c r="E31">
         <v>4.7530599999999996</v>
       </c>
+      <c r="F31">
+        <v>0.98013499999999998</v>
+      </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>32</v>
       </c>
@@ -12623,8 +12703,11 @@
       <c r="E32">
         <v>3.4933740000000002</v>
       </c>
+      <c r="F32">
+        <v>0.98258400000000001</v>
+      </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>64</v>
       </c>
@@ -12637,8 +12720,11 @@
       <c r="E33">
         <v>3.1794690000000001</v>
       </c>
+      <c r="F33">
+        <v>0.95097600000000004</v>
+      </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -12654,8 +12740,11 @@
       <c r="E35">
         <v>0.84752000000000005</v>
       </c>
+      <c r="F35">
+        <v>0.45594899999999999</v>
+      </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B36">
         <v>2</v>
       </c>
@@ -12668,8 +12757,11 @@
       <c r="E36">
         <v>1.564548</v>
       </c>
+      <c r="F36">
+        <v>0.75457700000000005</v>
+      </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>4</v>
       </c>
@@ -12682,8 +12774,11 @@
       <c r="E37">
         <v>2.6789260000000001</v>
       </c>
+      <c r="F37">
+        <v>1.0737639999999999</v>
+      </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>8</v>
       </c>
@@ -12696,8 +12791,11 @@
       <c r="E38">
         <v>4.1311869999999997</v>
       </c>
+      <c r="F38">
+        <v>1.1371290000000001</v>
+      </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>16</v>
       </c>
@@ -12710,8 +12808,11 @@
       <c r="E39">
         <v>6.0910450000000003</v>
       </c>
+      <c r="F39">
+        <v>1.0699689999999999</v>
+      </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>32</v>
       </c>
@@ -12724,8 +12825,11 @@
       <c r="E40">
         <v>3.7800600000000002</v>
       </c>
+      <c r="F40">
+        <v>1.0421609999999999</v>
+      </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>64</v>
       </c>
@@ -12737,6 +12841,9 @@
       </c>
       <c r="E41">
         <v>3.5267590000000002</v>
+      </c>
+      <c r="F41">
+        <v>1.0362199999999999</v>
       </c>
     </row>
   </sheetData>
@@ -12754,8 +12861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13804,7 +13911,7 @@
         <v>0.66237800000000002</v>
       </c>
       <c r="F59">
-        <v>0.48161399999999999</v>
+        <v>0.43965500000000002</v>
       </c>
       <c r="G59">
         <v>0.22300900000000001</v>
@@ -13824,7 +13931,7 @@
         <v>1.287655</v>
       </c>
       <c r="F60">
-        <v>0.84786300000000003</v>
+        <v>0.79086900000000004</v>
       </c>
       <c r="G60">
         <v>0.42497099999999999</v>
@@ -13844,7 +13951,7 @@
         <v>2.2558590000000001</v>
       </c>
       <c r="F61">
-        <v>1.446753</v>
+        <v>1.42069</v>
       </c>
       <c r="G61">
         <v>0.61724500000000004</v>
@@ -13864,7 +13971,7 @@
         <v>3.2683520000000001</v>
       </c>
       <c r="F62">
-        <v>1.9671179999999999</v>
+        <v>1.837367</v>
       </c>
       <c r="G62">
         <v>1.2773209999999999</v>
@@ -13884,7 +13991,7 @@
         <v>5.600752</v>
       </c>
       <c r="F63">
-        <v>1.9432689999999999</v>
+        <v>1.9172210000000001</v>
       </c>
       <c r="G63">
         <v>1.6862280000000001</v>
@@ -13904,7 +14011,7 @@
         <v>3.4295620000000002</v>
       </c>
       <c r="F64">
-        <v>1.9125559999999999</v>
+        <v>1.903195</v>
       </c>
       <c r="G64">
         <v>1.7489870000000001</v>
@@ -13924,7 +14031,7 @@
         <v>3.2534969999999999</v>
       </c>
       <c r="F65">
-        <v>1.9091959999999999</v>
+        <v>1.9467669999999999</v>
       </c>
       <c r="G65">
         <v>1.683343</v>

</xml_diff>

<commit_message>
All plots until now
</commit_message>
<xml_diff>
--- a/src/Speedup Plots.xlsx
+++ b/src/Speedup Plots.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13763" yWindow="0" windowWidth="25598" windowHeight="14798" activeTab="1"/>
+    <workbookView xWindow="13763" yWindow="0" windowWidth="25598" windowHeight="14798"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>30% Delete</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>load factor: 20</t>
+  </si>
+  <si>
+    <t>16 Thread Speedups</t>
+  </si>
+  <si>
+    <t>Load Factor</t>
+  </si>
+  <si>
+    <t>Speedup</t>
   </si>
 </sst>
 </file>
@@ -192,6 +201,725 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>16 Thread Speedup for Varied Load Factors</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequential</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$4:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$4:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-01A1-491C-B673-24D38C8E3E0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Fine Grained</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$10:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$10:$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.56602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1716889999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.619192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.770651</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0794160000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-01A1-491C-B673-24D38C8E3E0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Memory Leak</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$16:$J$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$16:$K$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.9436779999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2766229999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9700810000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7530599999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0910450000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-01A1-491C-B673-24D38C8E3E0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>DCAS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$22:$J$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$22:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.71130199999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2324790000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91234599999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98013499999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0699689999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-01A1-491C-B673-24D38C8E3E0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Hazard Pointers</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$28:$J$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$28:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.7121569999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4776100000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3310960000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1908339999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.132503</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-01A1-491C-B673-24D38C8E3E0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="441437328"/>
+        <c:axId val="441430440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="441437328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Load Factor</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441430440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="441430440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441437328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1100,7 +1828,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1963,7 +2691,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2826,7 +3554,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3689,7 +4417,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4552,7 +5280,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5415,7 +6143,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6283,7 +7011,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -11603,6 +12331,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209552</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>716758</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FA21404-3234-4F16-B1CE-43953CF5BB67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>321468</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -12201,10 +12970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12213,13 +12982,13 @@
     <col min="2" max="2" width="6.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
@@ -12235,8 +13004,11 @@
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -12255,8 +13027,17 @@
       <c r="F3">
         <v>0.28692299999999998</v>
       </c>
+      <c r="G3">
+        <v>0.26746700000000001</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>2</v>
       </c>
@@ -12272,8 +13053,20 @@
       <c r="F4">
         <v>0.44977200000000001</v>
       </c>
+      <c r="G4">
+        <v>0.398121</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>4</v>
       </c>
@@ -12289,8 +13082,17 @@
       <c r="F5">
         <v>0.55448299999999995</v>
       </c>
+      <c r="G5">
+        <v>0.574797</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>8</v>
       </c>
@@ -12306,8 +13108,17 @@
       <c r="F6">
         <v>0.70880799999999999</v>
       </c>
+      <c r="G6">
+        <v>0.88993599999999995</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>16</v>
       </c>
@@ -12323,8 +13134,17 @@
       <c r="F7">
         <v>0.71130199999999999</v>
       </c>
+      <c r="G7">
+        <v>1.7121569999999999</v>
+      </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>32</v>
       </c>
@@ -12340,8 +13160,17 @@
       <c r="F8">
         <v>0.717916</v>
       </c>
+      <c r="G8">
+        <v>1.5535099999999999</v>
+      </c>
+      <c r="J8">
+        <v>20</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>64</v>
       </c>
@@ -12357,8 +13186,22 @@
       <c r="F9">
         <v>0.71992500000000004</v>
       </c>
+      <c r="G9">
+        <v>1.621651</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>3.56602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -12377,8 +13220,17 @@
       <c r="F11">
         <v>0.55763499999999999</v>
       </c>
+      <c r="G11">
+        <v>0.24599699999999999</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>4.1716889999999998</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>2</v>
       </c>
@@ -12394,8 +13246,17 @@
       <c r="F12">
         <v>0.73817500000000003</v>
       </c>
+      <c r="G12">
+        <v>0.33677299999999999</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>4.619192</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>4</v>
       </c>
@@ -12411,8 +13272,17 @@
       <c r="F13">
         <v>1.215751</v>
       </c>
+      <c r="G13">
+        <v>0.53374500000000002</v>
+      </c>
+      <c r="J13">
+        <v>15</v>
+      </c>
+      <c r="K13">
+        <v>4.770651</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>8</v>
       </c>
@@ -12428,8 +13298,17 @@
       <c r="F14">
         <v>1.302767</v>
       </c>
+      <c r="G14">
+        <v>0.90641799999999995</v>
+      </c>
+      <c r="J14">
+        <v>20</v>
+      </c>
+      <c r="K14">
+        <v>5.0794160000000002</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>16</v>
       </c>
@@ -12445,8 +13324,11 @@
       <c r="F15">
         <v>1.2324790000000001</v>
       </c>
+      <c r="G15">
+        <v>1.4776100000000001</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>32</v>
       </c>
@@ -12462,8 +13344,20 @@
       <c r="F16">
         <v>1.2296640000000001</v>
       </c>
+      <c r="G16">
+        <v>1.3372869999999999</v>
+      </c>
+      <c r="I16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>3.9436779999999998</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>64</v>
       </c>
@@ -12479,8 +13373,25 @@
       <c r="F17">
         <v>1.205122</v>
       </c>
+      <c r="G17">
+        <v>1.5250109999999999</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>4.2766229999999998</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="J18">
+        <v>10</v>
+      </c>
+      <c r="K18">
+        <v>4.9700810000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -12499,8 +13410,17 @@
       <c r="F19">
         <v>0.37883600000000001</v>
       </c>
+      <c r="G19">
+        <v>0.22255</v>
+      </c>
+      <c r="J19">
+        <v>15</v>
+      </c>
+      <c r="K19">
+        <v>4.7530599999999996</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>2</v>
       </c>
@@ -12516,8 +13436,17 @@
       <c r="F20">
         <v>0.59200399999999997</v>
       </c>
+      <c r="G20">
+        <v>0.339416</v>
+      </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
+      <c r="K20">
+        <v>6.0910450000000003</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>4</v>
       </c>
@@ -12533,8 +13462,11 @@
       <c r="F21">
         <v>0.874089</v>
       </c>
+      <c r="G21">
+        <v>0.52208900000000003</v>
+      </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>8</v>
       </c>
@@ -12550,8 +13482,20 @@
       <c r="F22">
         <v>0.90456199999999998</v>
       </c>
+      <c r="G22">
+        <v>0.73115300000000005</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0.71130199999999999</v>
+      </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>16</v>
       </c>
@@ -12567,8 +13511,17 @@
       <c r="F23">
         <v>0.91234599999999999</v>
       </c>
+      <c r="G23">
+        <v>1.3310960000000001</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>1.2324790000000001</v>
+      </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>32</v>
       </c>
@@ -12584,8 +13537,17 @@
       <c r="F24">
         <v>0.91863600000000001</v>
       </c>
+      <c r="G24">
+        <v>1.2719009999999999</v>
+      </c>
+      <c r="J24">
+        <v>10</v>
+      </c>
+      <c r="K24">
+        <v>0.91234599999999999</v>
+      </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>64</v>
       </c>
@@ -12601,8 +13563,25 @@
       <c r="F25">
         <v>0.92056300000000002</v>
       </c>
+      <c r="G25">
+        <v>1.396692</v>
+      </c>
+      <c r="J25">
+        <v>15</v>
+      </c>
+      <c r="K25">
+        <v>0.98013499999999998</v>
+      </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="J26">
+        <v>20</v>
+      </c>
+      <c r="K26">
+        <v>1.0699689999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -12621,8 +13600,11 @@
       <c r="F27">
         <v>0.41204000000000002</v>
       </c>
+      <c r="G27">
+        <v>0.187806</v>
+      </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>2</v>
       </c>
@@ -12638,8 +13620,20 @@
       <c r="F28">
         <v>0.51643099999999997</v>
       </c>
+      <c r="G28">
+        <v>0.27198499999999998</v>
+      </c>
+      <c r="I28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1.7121569999999999</v>
+      </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>4</v>
       </c>
@@ -12655,8 +13649,17 @@
       <c r="F29">
         <v>0.75488599999999995</v>
       </c>
+      <c r="G29">
+        <v>0.44139699999999998</v>
+      </c>
+      <c r="J29">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>1.4776100000000001</v>
+      </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>8</v>
       </c>
@@ -12672,8 +13675,17 @@
       <c r="F30">
         <v>0.98655000000000004</v>
       </c>
+      <c r="G30">
+        <v>0.72203799999999996</v>
+      </c>
+      <c r="J30">
+        <v>10</v>
+      </c>
+      <c r="K30">
+        <v>1.3310960000000001</v>
+      </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>16</v>
       </c>
@@ -12689,8 +13701,17 @@
       <c r="F31">
         <v>0.98013499999999998</v>
       </c>
+      <c r="G31">
+        <v>1.1908339999999999</v>
+      </c>
+      <c r="J31">
+        <v>15</v>
+      </c>
+      <c r="K31">
+        <v>1.1908339999999999</v>
+      </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>32</v>
       </c>
@@ -12706,8 +13727,17 @@
       <c r="F32">
         <v>0.98258400000000001</v>
       </c>
+      <c r="G32">
+        <v>1.2680499999999999</v>
+      </c>
+      <c r="J32">
+        <v>20</v>
+      </c>
+      <c r="K32">
+        <v>1.132503</v>
+      </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>64</v>
       </c>
@@ -12723,8 +13753,11 @@
       <c r="F33">
         <v>0.95097600000000004</v>
       </c>
+      <c r="G33">
+        <v>1.3938820000000001</v>
+      </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -12743,8 +13776,11 @@
       <c r="F35">
         <v>0.45594899999999999</v>
       </c>
+      <c r="G35">
+        <v>0.20208499999999999</v>
+      </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B36">
         <v>2</v>
       </c>
@@ -12760,8 +13796,11 @@
       <c r="F36">
         <v>0.75457700000000005</v>
       </c>
+      <c r="G36">
+        <v>0.31408199999999997</v>
+      </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>4</v>
       </c>
@@ -12777,8 +13816,11 @@
       <c r="F37">
         <v>1.0737639999999999</v>
       </c>
+      <c r="G37">
+        <v>0.45687</v>
+      </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>8</v>
       </c>
@@ -12794,8 +13836,11 @@
       <c r="F38">
         <v>1.1371290000000001</v>
       </c>
+      <c r="G38">
+        <v>0.68855699999999997</v>
+      </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>16</v>
       </c>
@@ -12811,8 +13856,11 @@
       <c r="F39">
         <v>1.0699689999999999</v>
       </c>
+      <c r="G39">
+        <v>1.132503</v>
+      </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>32</v>
       </c>
@@ -12828,8 +13876,11 @@
       <c r="F40">
         <v>1.0421609999999999</v>
       </c>
+      <c r="G40">
+        <v>1.2299500000000001</v>
+      </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>64</v>
       </c>
@@ -12844,11 +13895,15 @@
       </c>
       <c r="F41">
         <v>1.0362199999999999</v>
+      </c>
+      <c r="G41">
+        <v>1.185093</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -12861,7 +13916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="C3" workbookViewId="0">
       <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added average time per operation test
</commit_message>
<xml_diff>
--- a/src/Speedup Plots.xlsx
+++ b/src/Speedup Plots.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="25600" windowHeight="14800"/>
+    <workbookView xWindow="440" yWindow="0" windowWidth="25600" windowHeight="14800" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Load Factors" sheetId="2" r:id="rId1"/>
+    <sheet name="Performance" sheetId="1" r:id="rId2"/>
+    <sheet name="Average CPU Times" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>30% Delete</t>
   </si>
@@ -93,6 +94,27 @@
   <si>
     <t>Speedup</t>
   </si>
+  <si>
+    <t>Average CPU Times</t>
+  </si>
+  <si>
+    <t>inserts</t>
+  </si>
+  <si>
+    <t>deletes</t>
+  </si>
+  <si>
+    <t>lookups</t>
+  </si>
+  <si>
+    <t>Load factor: 5</t>
+  </si>
+  <si>
+    <t>Load factor: 10</t>
+  </si>
+  <si>
+    <t>Load factor: 1</t>
+  </si>
 </sst>
 </file>
 
@@ -148,8 +170,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -167,19 +209,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -283,7 +345,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$J$4:$J$8</c:f>
+              <c:f>'Load Factors'!$J$4:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -307,7 +369,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$K$4:$K$8</c:f>
+              <c:f>'Load Factors'!$K$4:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -368,7 +430,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$J$10:$J$14</c:f>
+              <c:f>'Load Factors'!$J$10:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -392,7 +454,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$K$10:$K$14</c:f>
+              <c:f>'Load Factors'!$K$10:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -453,7 +515,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$J$16:$J$20</c:f>
+              <c:f>'Load Factors'!$J$16:$J$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -477,7 +539,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$K$16:$K$20</c:f>
+              <c:f>'Load Factors'!$K$16:$K$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -491,7 +553,7 @@
                   <c:v>4.970081</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.75306</c:v>
+                  <c:v>5.482237</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6.091045</c:v>
@@ -538,7 +600,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$J$22:$J$26</c:f>
+              <c:f>'Load Factors'!$J$22:$J$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -562,7 +624,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$K$22:$K$26</c:f>
+              <c:f>'Load Factors'!$K$22:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -570,7 +632,7 @@
                   <c:v>0.711302</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.232479</c:v>
+                  <c:v>0.816864</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.912346</c:v>
@@ -623,7 +685,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$J$28:$J$32</c:f>
+              <c:f>'Load Factors'!$J$28:$J$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -647,7 +709,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$K$28:$K$32</c:f>
+              <c:f>'Load Factors'!$K$28:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -684,11 +746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2144042504"/>
-        <c:axId val="2145389416"/>
+        <c:axId val="2125581960"/>
+        <c:axId val="2144585448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2144042504"/>
+        <c:axId val="2125581960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,12 +829,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145389416"/>
+        <c:crossAx val="2144585448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145389416"/>
+        <c:axId val="2144585448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -859,7 +921,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144042504"/>
+        <c:crossAx val="2125581960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -984,7 +1046,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Performance!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1019,7 +1081,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Performance!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1049,7 +1111,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:f>Performance!$C$3:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1089,7 +1151,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Performance!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1124,7 +1186,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Performance!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1154,7 +1216,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$9</c:f>
+              <c:f>Performance!$D$3:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1194,7 +1256,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Performance!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1229,7 +1291,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Performance!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1259,7 +1321,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$9</c:f>
+              <c:f>Performance!$E$3:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1299,7 +1361,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>Performance!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1334,7 +1396,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Performance!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1364,7 +1426,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$9</c:f>
+              <c:f>Performance!$F$3:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1404,7 +1466,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Performance!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1439,7 +1501,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Performance!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1469,7 +1531,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$9</c:f>
+              <c:f>Performance!$G$3:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1512,11 +1574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2125507112"/>
-        <c:axId val="2128046664"/>
+        <c:axId val="2145217656"/>
+        <c:axId val="2109654536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2125507112"/>
+        <c:axId val="2145217656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -1597,13 +1659,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128046664"/>
+        <c:crossAx val="2109654536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128046664"/>
+        <c:axId val="2109654536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1690,7 +1752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125507112"/>
+        <c:crossAx val="2145217656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1859,7 +1921,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:f>Performance!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1889,7 +1951,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$11:$C$17</c:f>
+              <c:f>Performance!$C$11:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1956,7 +2018,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:f>Performance!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1986,7 +2048,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$11:$D$17</c:f>
+              <c:f>Performance!$D$11:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2053,7 +2115,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:f>Performance!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2083,7 +2145,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$11:$E$17</c:f>
+              <c:f>Performance!$E$11:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2150,7 +2212,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:f>Performance!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2180,7 +2242,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$11:$F$17</c:f>
+              <c:f>Performance!$F$11:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2247,7 +2309,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$B$17</c:f>
+              <c:f>Performance!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2277,7 +2339,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$11:$G$17</c:f>
+              <c:f>Performance!$G$11:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2320,11 +2382,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2031041320"/>
-        <c:axId val="2125067720"/>
+        <c:axId val="2144945112"/>
+        <c:axId val="2145157032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2031041320"/>
+        <c:axId val="2144945112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -2404,13 +2466,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125067720"/>
+        <c:crossAx val="2145157032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2125067720"/>
+        <c:axId val="2145157032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2559,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2031041320"/>
+        <c:crossAx val="2144945112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2666,7 +2728,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$25</c:f>
+              <c:f>Performance!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2696,7 +2758,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$25</c:f>
+              <c:f>Performance!$C$19:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2763,7 +2825,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$25</c:f>
+              <c:f>Performance!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2793,7 +2855,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$25</c:f>
+              <c:f>Performance!$D$19:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2860,7 +2922,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$25</c:f>
+              <c:f>Performance!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2890,7 +2952,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$19:$E$25</c:f>
+              <c:f>Performance!$E$19:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2957,7 +3019,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$25</c:f>
+              <c:f>Performance!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2987,7 +3049,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$19:$F$25</c:f>
+              <c:f>Performance!$F$19:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3054,7 +3116,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$25</c:f>
+              <c:f>Performance!$B$19:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3084,7 +3146,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$25</c:f>
+              <c:f>Performance!$G$19:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3127,11 +3189,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2129557112"/>
-        <c:axId val="2128898264"/>
+        <c:axId val="2128156344"/>
+        <c:axId val="2145337768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2129557112"/>
+        <c:axId val="2128156344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -3211,13 +3273,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128898264"/>
+        <c:crossAx val="2145337768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128898264"/>
+        <c:axId val="2145337768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3304,7 +3366,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2129557112"/>
+        <c:crossAx val="2128156344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3473,7 +3535,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$B$33</c:f>
+              <c:f>Performance!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3503,7 +3565,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$27:$C$33</c:f>
+              <c:f>Performance!$C$27:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3570,7 +3632,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$B$33</c:f>
+              <c:f>Performance!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3600,7 +3662,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$27:$D$33</c:f>
+              <c:f>Performance!$D$27:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3667,7 +3729,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$B$33</c:f>
+              <c:f>Performance!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3697,7 +3759,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$27:$E$33</c:f>
+              <c:f>Performance!$E$27:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3764,7 +3826,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$B$33</c:f>
+              <c:f>Performance!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3794,7 +3856,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$27:$F$33</c:f>
+              <c:f>Performance!$F$27:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3861,7 +3923,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$B$33</c:f>
+              <c:f>Performance!$B$27:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3891,7 +3953,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$27:$G$33</c:f>
+              <c:f>Performance!$G$27:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3934,11 +3996,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2097086216"/>
-        <c:axId val="2130420728"/>
+        <c:axId val="2031193432"/>
+        <c:axId val="2123144696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2097086216"/>
+        <c:axId val="2031193432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -4018,13 +4080,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130420728"/>
+        <c:crossAx val="2123144696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2130420728"/>
+        <c:axId val="2123144696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4111,7 +4173,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2097086216"/>
+        <c:crossAx val="2031193432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4280,7 +4342,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$B$41</c:f>
+              <c:f>Performance!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4310,7 +4372,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$35:$C$41</c:f>
+              <c:f>Performance!$C$35:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4377,7 +4439,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$B$41</c:f>
+              <c:f>Performance!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4407,7 +4469,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$35:$D$41</c:f>
+              <c:f>Performance!$D$35:$D$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4474,7 +4536,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$B$41</c:f>
+              <c:f>Performance!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4504,7 +4566,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$35:$E$41</c:f>
+              <c:f>Performance!$E$35:$E$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4571,7 +4633,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$B$41</c:f>
+              <c:f>Performance!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4601,7 +4663,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$35:$F$41</c:f>
+              <c:f>Performance!$F$35:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4668,7 +4730,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$B$41</c:f>
+              <c:f>Performance!$B$35:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4698,7 +4760,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$35:$G$41</c:f>
+              <c:f>Performance!$G$35:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -4741,11 +4803,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2144981624"/>
-        <c:axId val="2144440136"/>
+        <c:axId val="2124899096"/>
+        <c:axId val="2124672408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2144981624"/>
+        <c:axId val="2124899096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -4825,13 +4887,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144440136"/>
+        <c:crossAx val="2124672408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2144440136"/>
+        <c:axId val="2124672408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4918,7 +4980,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144981624"/>
+        <c:crossAx val="2124899096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5087,7 +5149,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5117,7 +5179,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$43:$C$49</c:f>
+              <c:f>Performance!$C$43:$C$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5184,7 +5246,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5214,7 +5276,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$43:$D$49</c:f>
+              <c:f>Performance!$D$43:$D$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5281,7 +5343,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5311,7 +5373,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$43:$E$49</c:f>
+              <c:f>Performance!$E$43:$E$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5378,7 +5440,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5408,7 +5470,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$43:$F$49</c:f>
+              <c:f>Performance!$F$43:$F$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5475,7 +5537,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5505,7 +5567,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$43:$G$49</c:f>
+              <c:f>Performance!$G$43:$G$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5548,11 +5610,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2130096312"/>
-        <c:axId val="2145630360"/>
+        <c:axId val="2145070424"/>
+        <c:axId val="2144685688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2130096312"/>
+        <c:axId val="2145070424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -5632,13 +5694,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145630360"/>
+        <c:crossAx val="2144685688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145630360"/>
+        <c:axId val="2144685688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5725,7 +5787,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130096312"/>
+        <c:crossAx val="2145070424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5899,7 +5961,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5929,7 +5991,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$51:$C$57</c:f>
+              <c:f>Performance!$C$51:$C$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5996,7 +6058,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6026,7 +6088,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$51:$D$57</c:f>
+              <c:f>Performance!$D$51:$D$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6093,7 +6155,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6123,7 +6185,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$51:$E$57</c:f>
+              <c:f>Performance!$E$51:$E$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6190,7 +6252,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6220,7 +6282,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$51:$F$57</c:f>
+              <c:f>Performance!$F$51:$F$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6287,7 +6349,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6317,7 +6379,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$51:$G$57</c:f>
+              <c:f>Performance!$G$51:$G$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6360,11 +6422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2144113576"/>
-        <c:axId val="2145471816"/>
+        <c:axId val="2144531736"/>
+        <c:axId val="2144605032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2144113576"/>
+        <c:axId val="2144531736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -6444,13 +6506,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145471816"/>
+        <c:crossAx val="2144605032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145471816"/>
+        <c:axId val="2144605032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6537,7 +6599,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144113576"/>
+        <c:crossAx val="2144531736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6711,7 +6773,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6741,7 +6803,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$59:$C$65</c:f>
+              <c:f>Performance!$C$59:$C$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6808,7 +6870,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6838,7 +6900,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$59:$D$65</c:f>
+              <c:f>Performance!$D$59:$D$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6905,7 +6967,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6935,7 +6997,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$59:$E$65</c:f>
+              <c:f>Performance!$E$59:$E$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7002,7 +7064,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7032,7 +7094,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$59:$F$65</c:f>
+              <c:f>Performance!$F$59:$F$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7099,7 +7161,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$49</c:f>
+              <c:f>Performance!$B$43:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7129,7 +7191,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$59:$G$65</c:f>
+              <c:f>Performance!$G$59:$G$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7172,11 +7234,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2145983128"/>
-        <c:axId val="2145991752"/>
+        <c:axId val="2145270568"/>
+        <c:axId val="2144760408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2145983128"/>
+        <c:axId val="2145270568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65.0"/>
@@ -7256,13 +7318,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145991752"/>
+        <c:crossAx val="2144760408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145991752"/>
+        <c:axId val="2144760408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7349,7 +7411,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145983128"/>
+        <c:crossAx val="2145270568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12523,8 +12585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -12770,7 +12832,7 @@
         <v>0.77187700000000004</v>
       </c>
       <c r="F11">
-        <v>0.55763499999999999</v>
+        <v>0.32731100000000002</v>
       </c>
       <c r="G11">
         <v>0.26589000000000002</v>
@@ -12797,7 +12859,7 @@
         <v>1.2931170000000001</v>
       </c>
       <c r="F12">
-        <v>0.73817500000000003</v>
+        <v>0.52477700000000005</v>
       </c>
       <c r="G12">
         <v>0.437554</v>
@@ -12824,7 +12886,7 @@
         <v>2.2189830000000001</v>
       </c>
       <c r="F13">
-        <v>1.215751</v>
+        <v>0.78607199999999999</v>
       </c>
       <c r="G13">
         <v>0.56104200000000004</v>
@@ -12851,7 +12913,7 @@
         <v>3.2570480000000002</v>
       </c>
       <c r="F14">
-        <v>1.302767</v>
+        <v>0.83149700000000004</v>
       </c>
       <c r="G14">
         <v>1.302338</v>
@@ -12878,7 +12940,7 @@
         <v>4.2766229999999998</v>
       </c>
       <c r="F15">
-        <v>1.2324790000000001</v>
+        <v>0.81686400000000003</v>
       </c>
       <c r="G15">
         <v>2.1860789999999999</v>
@@ -12898,7 +12960,7 @@
         <v>3.1607340000000002</v>
       </c>
       <c r="F16">
-        <v>1.2296640000000001</v>
+        <v>0.79300199999999998</v>
       </c>
       <c r="G16">
         <v>1.685362</v>
@@ -12928,7 +12990,7 @@
         <v>2.8426230000000001</v>
       </c>
       <c r="F17">
-        <v>1.205122</v>
+        <v>0.78582099999999999</v>
       </c>
       <c r="G17">
         <v>1.6644559999999999</v>
@@ -12976,8 +13038,7 @@
         <v>15</v>
       </c>
       <c r="K19">
-        <f>E31</f>
-        <v>4.7530599999999996</v>
+        <v>5.4822369999999996</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -13081,7 +13142,7 @@
       </c>
       <c r="K23">
         <f>F15</f>
-        <v>1.2324790000000001</v>
+        <v>0.81686400000000003</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -13487,8 +13548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14673,4 +14734,1181 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.35943399999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.42527700000000002</v>
+      </c>
+      <c r="G4">
+        <v>0.70542099999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.52338799999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.49354999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.93481800000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.63755099999999998</v>
+      </c>
+      <c r="E6">
+        <v>1.5051600000000001</v>
+      </c>
+      <c r="G6">
+        <v>1.635742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>5.7264499999999998</v>
+      </c>
+      <c r="E7">
+        <v>6.9330879999999997</v>
+      </c>
+      <c r="G7">
+        <v>6.0713309999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>12.780386999999999</v>
+      </c>
+      <c r="E8">
+        <v>11.145113</v>
+      </c>
+      <c r="G8">
+        <v>16.058009999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>12.53213</v>
+      </c>
+      <c r="E9">
+        <v>18.201039000000002</v>
+      </c>
+      <c r="G9">
+        <v>30.877390999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10">
+        <v>64</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>15.021520000000001</v>
+      </c>
+      <c r="E10">
+        <v>18.808657</v>
+      </c>
+      <c r="G10">
+        <v>18.926735000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.296956</v>
+      </c>
+      <c r="E12">
+        <v>0.39329399999999998</v>
+      </c>
+      <c r="G12">
+        <v>0.96951600000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0.49830000000000002</v>
+      </c>
+      <c r="E13">
+        <v>0.42638999999999999</v>
+      </c>
+      <c r="G13">
+        <v>1.116619</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0.34949200000000002</v>
+      </c>
+      <c r="E14">
+        <v>0.59093200000000001</v>
+      </c>
+      <c r="G14">
+        <v>1.3370340000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0.41226499999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.53278099999999995</v>
+      </c>
+      <c r="G15">
+        <v>1.435764</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0.51988800000000002</v>
+      </c>
+      <c r="E16">
+        <v>0.48691800000000002</v>
+      </c>
+      <c r="G16">
+        <v>1.1587959999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0.40026699999999998</v>
+      </c>
+      <c r="E17">
+        <v>0.51380300000000001</v>
+      </c>
+      <c r="G17">
+        <v>1.19404</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18">
+        <v>64</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.45822099999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.55782299999999996</v>
+      </c>
+      <c r="G18">
+        <v>1.3964909999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0.29127500000000001</v>
+      </c>
+      <c r="E20">
+        <v>0.34417399999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.71916599999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.45919700000000002</v>
+      </c>
+      <c r="E21">
+        <v>0.38795600000000002</v>
+      </c>
+      <c r="G21">
+        <v>0.84111199999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.41846499999999998</v>
+      </c>
+      <c r="E22">
+        <v>0.519374</v>
+      </c>
+      <c r="G22">
+        <v>1.0557570000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.432896</v>
+      </c>
+      <c r="E23">
+        <v>0.47303200000000001</v>
+      </c>
+      <c r="G23">
+        <v>1.107702</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0.41407300000000002</v>
+      </c>
+      <c r="E24">
+        <v>0.41251300000000002</v>
+      </c>
+      <c r="G24">
+        <v>0.8659</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0.41356900000000002</v>
+      </c>
+      <c r="E25">
+        <v>0.46469700000000003</v>
+      </c>
+      <c r="G25">
+        <v>1.0179910000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26">
+        <v>64</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0.56731699999999996</v>
+      </c>
+      <c r="E26">
+        <v>0.54564500000000005</v>
+      </c>
+      <c r="G26">
+        <v>1.2956160000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0.48986400000000002</v>
+      </c>
+      <c r="E28">
+        <v>0.45796100000000001</v>
+      </c>
+      <c r="G28">
+        <v>1.0551280000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0.507718</v>
+      </c>
+      <c r="E29">
+        <v>0.67778400000000005</v>
+      </c>
+      <c r="G29">
+        <v>1.094303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.81154000000000004</v>
+      </c>
+      <c r="E30">
+        <v>0.94021900000000003</v>
+      </c>
+      <c r="G30">
+        <v>1.4626680000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>4.2800700000000003</v>
+      </c>
+      <c r="E31">
+        <v>6.758991</v>
+      </c>
+      <c r="G31">
+        <v>6.0771309999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="B32">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>10.198767</v>
+      </c>
+      <c r="E32">
+        <v>16.723860999999999</v>
+      </c>
+      <c r="G32">
+        <v>20.927690999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>12.028587999999999</v>
+      </c>
+      <c r="E33">
+        <v>23.957877</v>
+      </c>
+      <c r="G33">
+        <v>43.136282999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="B34">
+        <v>64</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>18.291945999999999</v>
+      </c>
+      <c r="E34">
+        <v>16.704646</v>
+      </c>
+      <c r="G34">
+        <v>23.588799999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0.40503299999999998</v>
+      </c>
+      <c r="E36">
+        <v>0.44432100000000002</v>
+      </c>
+      <c r="G36">
+        <v>1.0793680000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0.34977599999999998</v>
+      </c>
+      <c r="E37">
+        <v>0.48507299999999998</v>
+      </c>
+      <c r="G37">
+        <v>1.289609</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0.549238</v>
+      </c>
+      <c r="E38">
+        <v>0.52694700000000005</v>
+      </c>
+      <c r="G38">
+        <v>2.1390950000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0.41424699999999998</v>
+      </c>
+      <c r="E39">
+        <v>0.53190000000000004</v>
+      </c>
+      <c r="G39">
+        <v>2.0542479999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="B40">
+        <v>16</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.38673600000000002</v>
+      </c>
+      <c r="E40">
+        <v>0.55158300000000005</v>
+      </c>
+      <c r="G40">
+        <v>1.4369019999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="B41">
+        <v>32</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0.44172499999999998</v>
+      </c>
+      <c r="E41">
+        <v>0.57439099999999998</v>
+      </c>
+      <c r="G41">
+        <v>1.3701140000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="B42">
+        <v>64</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0.53883800000000004</v>
+      </c>
+      <c r="E42">
+        <v>0.66780099999999998</v>
+      </c>
+      <c r="G42">
+        <v>1.5910850000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>0.39637499999999998</v>
+      </c>
+      <c r="E44">
+        <v>0.39255699999999999</v>
+      </c>
+      <c r="G44">
+        <v>1.0145360000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0.43377900000000003</v>
+      </c>
+      <c r="E45">
+        <v>0.54172100000000001</v>
+      </c>
+      <c r="G45">
+        <v>1.0050410000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0.53964800000000002</v>
+      </c>
+      <c r="E46">
+        <v>0.54218999999999995</v>
+      </c>
+      <c r="G46">
+        <v>1.427233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="B47">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0.49271900000000002</v>
+      </c>
+      <c r="E47">
+        <v>0.504162</v>
+      </c>
+      <c r="G47">
+        <v>1.3790119999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="B48">
+        <v>16</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0.39069100000000001</v>
+      </c>
+      <c r="E48">
+        <v>0.50961500000000004</v>
+      </c>
+      <c r="G48">
+        <v>1.2065410000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="B49">
+        <v>32</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0.47419499999999998</v>
+      </c>
+      <c r="E49">
+        <v>0.46681699999999998</v>
+      </c>
+      <c r="G49">
+        <v>1.312389</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="B50">
+        <v>64</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>0.55952400000000002</v>
+      </c>
+      <c r="E50">
+        <v>0.50556299999999998</v>
+      </c>
+      <c r="G50">
+        <v>1.433359</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0.43536599999999998</v>
+      </c>
+      <c r="E52">
+        <v>0.57133500000000004</v>
+      </c>
+      <c r="G52">
+        <v>1.149294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0.62234100000000003</v>
+      </c>
+      <c r="E53">
+        <v>0.67979199999999995</v>
+      </c>
+      <c r="G53">
+        <v>1.752734</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>0.73226599999999997</v>
+      </c>
+      <c r="E54">
+        <v>1.4032530000000001</v>
+      </c>
+      <c r="G54">
+        <v>1.7654000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="B55">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>6.1730260000000001</v>
+      </c>
+      <c r="E55">
+        <v>7.0857359999999998</v>
+      </c>
+      <c r="G55">
+        <v>13.229831000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="B56">
+        <v>16</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>14.548584999999999</v>
+      </c>
+      <c r="E56">
+        <v>14.97377</v>
+      </c>
+      <c r="G56">
+        <v>28.180803000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="B57">
+        <v>32</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>11.527737999999999</v>
+      </c>
+      <c r="E57">
+        <v>17.299887999999999</v>
+      </c>
+      <c r="G57">
+        <v>41.61253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="B58">
+        <v>64</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>20.437244</v>
+      </c>
+      <c r="E58">
+        <v>16.178674999999998</v>
+      </c>
+      <c r="G58">
+        <v>27.210723999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>0.32774500000000001</v>
+      </c>
+      <c r="E60">
+        <v>0.46664</v>
+      </c>
+      <c r="G60">
+        <v>1.464399</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>0.51661699999999999</v>
+      </c>
+      <c r="E61">
+        <v>0.65880899999999998</v>
+      </c>
+      <c r="G61">
+        <v>1.8218259999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>0.40765800000000002</v>
+      </c>
+      <c r="E62">
+        <v>0.59867599999999999</v>
+      </c>
+      <c r="G62">
+        <v>1.907014</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="B63">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0.40539199999999997</v>
+      </c>
+      <c r="E63">
+        <v>0.67464299999999999</v>
+      </c>
+      <c r="G63">
+        <v>2.0248349999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="B64">
+        <v>16</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>0.48119200000000001</v>
+      </c>
+      <c r="E64">
+        <v>0.53624300000000003</v>
+      </c>
+      <c r="G64">
+        <v>2.0278909999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="B65">
+        <v>32</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>0.65607800000000005</v>
+      </c>
+      <c r="E65">
+        <v>0.61178299999999997</v>
+      </c>
+      <c r="G65">
+        <v>1.8820870000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="B66">
+        <v>64</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>0.55272200000000005</v>
+      </c>
+      <c r="E66">
+        <v>0.575681</v>
+      </c>
+      <c r="G66">
+        <v>2.5411419999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>0.37683</v>
+      </c>
+      <c r="E68">
+        <v>0.39878999999999998</v>
+      </c>
+      <c r="G68">
+        <v>1.0883149999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>0.41291099999999997</v>
+      </c>
+      <c r="E69">
+        <v>0.458841</v>
+      </c>
+      <c r="G69">
+        <v>1.5642849999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>0.37281399999999998</v>
+      </c>
+      <c r="E70">
+        <v>0.76437999999999995</v>
+      </c>
+      <c r="G70">
+        <v>1.5629649999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="B71">
+        <v>8</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0.40951500000000002</v>
+      </c>
+      <c r="E71">
+        <v>0.56870699999999996</v>
+      </c>
+      <c r="G71">
+        <v>1.6640200000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="B72">
+        <v>16</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>0.45288099999999998</v>
+      </c>
+      <c r="E72">
+        <v>0.47669699999999998</v>
+      </c>
+      <c r="G72">
+        <v>1.985449</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="B73">
+        <v>32</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0.59148999999999996</v>
+      </c>
+      <c r="E73">
+        <v>0.46444000000000002</v>
+      </c>
+      <c r="G73">
+        <v>1.7134469999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="B74">
+        <v>64</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>0.56408100000000005</v>
+      </c>
+      <c r="E74">
+        <v>0.68728999999999996</v>
+      </c>
+      <c r="G74">
+        <v>2.1649409999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>